<commit_message>
📊 Horarios actualizados Línea 141 - 1266
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:12:47</t>
+          <t>Última actualización: 02:38:35</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 2</t>
+          <t>Total filas: 3</t>
         </is>
       </c>
     </row>
@@ -478,21 +478,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>01:12:47</t>
+          <t>02:38:35</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>01:25</t>
+          <t>03:01</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -503,23 +503,48 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>01:12:47</t>
+          <t>02:38:35</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>03:02</t>
+          <t>03:48</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>02:38:35</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>04:02</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>84</v>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -554,7 +579,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:12:47</t>
+          <t>Última actualización: 02:38:35</t>
         </is>
       </c>
     </row>
@@ -594,7 +619,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:12:47</t>
+          <t>Última actualización: 02:38:35</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1267
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:38:35</t>
+          <t>Última actualización: 03:27:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 6</t>
         </is>
       </c>
     </row>
@@ -478,21 +478,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>02:38:35</t>
+          <t>03:27:48</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>03:01</t>
+          <t>03:48</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -503,21 +503,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>02:38:35</t>
+          <t>03:27:48</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -528,12 +528,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>02:38:35</t>
+          <t>03:27:48</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>04:02</t>
+          <t>04:47</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -542,9 +542,84 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>03:27:48</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>86</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>03:27:48</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>05:16</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>109</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>03:27:48</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>05:22</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>115</v>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -579,7 +654,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:38:35</t>
+          <t>Última actualización: 03:27:48</t>
         </is>
       </c>
     </row>
@@ -619,7 +694,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:38:35</t>
+          <t>Última actualización: 03:27:48</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1268
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:27:48</t>
+          <t>Última actualización: 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 6</t>
+          <t>Total filas: 8</t>
         </is>
       </c>
     </row>
@@ -478,21 +478,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>03:27:48</t>
+          <t>04:10:26</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>04:47</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -503,21 +503,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>03:27:48</t>
+          <t>04:10:26</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>04:53</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -528,21 +528,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>03:27:48</t>
+          <t>04:10:26</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>04:47</t>
+          <t>05:17</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -553,21 +553,21 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>03:27:48</t>
+          <t>04:10:26</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -578,21 +578,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>03:27:48</t>
+          <t>04:10:26</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -603,23 +603,73 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>03:27:48</t>
+          <t>04:10:26</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>05:47</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>04:10:26</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>06:01</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>111</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>04:10:26</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>06:09</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>119</v>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -654,7 +704,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:27:48</t>
+          <t>Última actualización: 04:10:26</t>
         </is>
       </c>
     </row>
@@ -694,7 +744,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:27:48</t>
+          <t>Última actualización: 04:10:26</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1269
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:10:26</t>
+          <t>Última actualización: 04:50:21</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 8</t>
+          <t>Total filas: 12</t>
         </is>
       </c>
     </row>
@@ -478,21 +478,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>04:10:26</t>
+          <t>04:50:21</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>04:47</t>
+          <t>04:53</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -503,21 +503,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>04:10:26</t>
+          <t>04:50:21</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>05:17</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -528,21 +528,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>04:10:26</t>
+          <t>04:50:21</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>05:17</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -553,21 +553,21 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>04:10:26</t>
+          <t>04:50:21</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -578,21 +578,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>04:10:26</t>
+          <t>04:50:21</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>05:44</t>
+          <t>05:47</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>94</v>
+        <v>57</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -603,21 +603,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>04:10:26</t>
+          <t>04:50:21</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>05:47</t>
+          <t>06:01</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -628,21 +628,21 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>04:10:26</t>
+          <t>04:50:21</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>06:01</t>
+          <t>06:09</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -653,23 +653,123 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>04:10:26</t>
+          <t>04:50:21</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>06:09</t>
+          <t>06:16</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>04:50:21</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>06:30</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>100</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>04:50:21</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>06:34</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>104</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>04:50:21</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>06:39</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>109</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>04:50:21</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>06:41</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>111</v>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -686,7 +786,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -704,14 +804,66 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:10:26</t>
+          <t>Última actualización: 04:50:21</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 0</t>
+          <t>Total filas: 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>04:50:21</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>06:16</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>86</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
         </is>
       </c>
     </row>
@@ -744,7 +896,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:10:26</t>
+          <t>Última actualización: 04:50:21</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1270
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:50:21</t>
+          <t>Última actualización: 05:01:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 12</t>
+          <t>Total filas: 13</t>
         </is>
       </c>
     </row>
@@ -478,21 +478,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>04:50:21</t>
+          <t>05:01:48</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -503,21 +503,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>04:50:21</t>
+          <t>05:01:48</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>05:17</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -528,21 +528,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>04:50:21</t>
+          <t>05:01:48</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -553,21 +553,21 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>04:50:21</t>
+          <t>05:01:48</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>05:44</t>
+          <t>05:46</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -578,21 +578,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>04:50:21</t>
+          <t>05:01:48</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>05:47</t>
+          <t>06:01</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -603,21 +603,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>04:50:21</t>
+          <t>05:01:48</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>06:01</t>
+          <t>06:09</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -628,21 +628,21 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>04:50:21</t>
+          <t>05:01:48</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>06:09</t>
+          <t>06:15</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -653,21 +653,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>04:50:21</t>
+          <t>05:01:48</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>06:16</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -678,21 +678,21 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>04:50:21</t>
+          <t>05:01:48</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:34</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -703,21 +703,21 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:50:21</t>
+          <t>05:01:48</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>06:34</t>
+          <t>06:38</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -728,21 +728,21 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>04:50:21</t>
+          <t>05:01:48</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>06:39</t>
+          <t>06:40</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,23 +753,48 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>04:50:21</t>
+          <t>05:01:48</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>06:41</t>
+          <t>06:56</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>05:01:48</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>06:59</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>118</v>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -786,7 +811,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -804,14 +829,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:50:21</t>
+          <t>Última actualización: 05:01:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 1</t>
+          <t>Total filas: 2</t>
         </is>
       </c>
     </row>
@@ -845,12 +870,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>04:50:21</t>
+          <t>05:01:48</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>06:16</t>
+          <t>06:15</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -859,9 +884,34 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>05:01:48</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>06:56</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>115</v>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -896,7 +946,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:50:21</t>
+          <t>Última actualización: 05:01:49</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1271
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:01:49</t>
+          <t>Última actualización: 05:47:29</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 13</t>
+          <t>Total filas: 16</t>
         </is>
       </c>
     </row>
@@ -478,12 +478,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>05:01:48</t>
+          <t>05:47:29</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>05:47</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -503,21 +503,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>05:01:48</t>
+          <t>05:47:29</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>06:09</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -528,21 +528,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>05:01:48</t>
+          <t>05:47:29</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>05:44</t>
+          <t>06:16</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -553,21 +553,21 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>05:01:48</t>
+          <t>05:47:29</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>05:46</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -578,21 +578,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>05:01:48</t>
+          <t>05:47:29</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>06:01</t>
+          <t>06:34</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -603,21 +603,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>05:01:48</t>
+          <t>05:47:29</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>06:09</t>
+          <t>06:39</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -628,21 +628,21 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>05:01:48</t>
+          <t>05:47:29</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>06:15</t>
+          <t>06:41</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -653,21 +653,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>05:01:48</t>
+          <t>05:47:29</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:57</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -678,21 +678,21 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>05:01:48</t>
+          <t>05:47:29</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>06:34</t>
+          <t>06:59</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -703,21 +703,21 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>05:01:48</t>
+          <t>05:47:29</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>06:38</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -728,21 +728,21 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:01:48</t>
+          <t>05:47:29</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>06:40</t>
+          <t>07:19</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,21 +753,21 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:01:48</t>
+          <t>05:47:29</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>06:56</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -778,23 +778,98 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>05:01:48</t>
+          <t>05:47:29</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>06:59</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>05:47:29</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>07:29</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>102</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>05:47:29</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>07:35</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>108</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>05:47:29</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>07:36</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>109</v>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -811,7 +886,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -829,14 +904,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:01:49</t>
+          <t>Última actualización: 05:47:29</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 2</t>
+          <t>Total filas: 3</t>
         </is>
       </c>
     </row>
@@ -870,12 +945,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>05:01:48</t>
+          <t>05:47:29</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>06:15</t>
+          <t>06:16</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -884,7 +959,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -895,12 +970,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>05:01:48</t>
+          <t>05:47:29</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>06:56</t>
+          <t>06:57</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -909,9 +984,34 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>05:47:29</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>07:15</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>88</v>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -928,7 +1028,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -946,14 +1046,66 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:01:49</t>
+          <t>Última actualización: 05:47:29</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 0</t>
+          <t>Total filas: 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>05:47:29</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>07:43</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>116</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1272
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:47:29</t>
+          <t>Última actualización: 06:15:23</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 16</t>
+          <t>Total filas: 22</t>
         </is>
       </c>
     </row>
@@ -528,7 +528,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>05:47:29</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -553,7 +553,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>05:47:29</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -578,7 +578,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>05:47:29</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>05:47:29</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -628,7 +628,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>05:47:29</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -653,7 +653,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>05:47:29</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -667,7 +667,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -678,7 +678,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>05:47:29</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -728,21 +728,21 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:47:29</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>07:19</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,21 +753,21 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:47:29</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:19</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -778,7 +778,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>05:47:29</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -788,11 +788,11 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -803,21 +803,21 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>05:47:29</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>07:29</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -828,21 +828,21 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>05:47:29</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>07:35</t>
+          <t>07:29</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -853,23 +853,173 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>06:15:23</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>07:35</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>80</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>05:47:29</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B22" t="inlineStr">
         <is>
           <t>07:36</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C22" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="D21" t="n">
+      <c r="D22" t="n">
         <v>109</v>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>06:15:23</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>07:37</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>82</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>06:15:23</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>07:55</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>100</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>06:15:23</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>105</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>06:15:23</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>08:11</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>116</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>06:15:23</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>08:13</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>118</v>
+      </c>
+      <c r="E27" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -886,7 +1036,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -904,14 +1054,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:47:29</t>
+          <t>Última actualización: 06:15:23</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 4</t>
         </is>
       </c>
     </row>
@@ -945,7 +1095,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>05:47:29</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -959,7 +1109,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -970,7 +1120,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>05:47:29</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -984,7 +1134,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1012,6 +1162,31 @@
         <v>88</v>
       </c>
       <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>06:15:23</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>07:16</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>61</v>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1046,7 +1221,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:47:29</t>
+          <t>Última actualización: 06:15:23</t>
         </is>
       </c>
     </row>
@@ -1087,7 +1262,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>05:47:29</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1101,7 +1276,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1273
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:15:23</t>
+          <t>Última actualización: 06:46:40</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 22</t>
+          <t>Total filas: 31</t>
         </is>
       </c>
     </row>
@@ -653,12 +653,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>06:57</t>
+          <t>06:56</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -667,7 +667,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -683,16 +683,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>06:59</t>
+          <t>06:57</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -703,21 +703,21 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>05:47:29</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>06:59</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>88</v>
+        <v>13</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -728,12 +728,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -758,16 +758,16 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>07:19</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -778,21 +778,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:19</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -803,21 +803,21 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:20</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -833,16 +833,16 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>07:29</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -853,21 +853,21 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>07:35</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -878,21 +878,21 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>05:47:29</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>07:36</t>
+          <t>07:29</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>109</v>
+        <v>43</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -903,21 +903,21 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>07:37</t>
+          <t>07:35</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -928,21 +928,21 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>07:55</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -958,16 +958,16 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>07:37</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -978,21 +978,21 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>08:11</t>
+          <t>07:43</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>116</v>
+        <v>57</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1003,23 +1003,248 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>07:55</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>69</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>06:46:40</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>74</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>06:46:40</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>08:01</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>75</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>06:46:40</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>08:06</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>80</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>06:46:40</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>08:11</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>85</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>06:46:40</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
           <t>08:13</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>15X38_ABASTO</t>
         </is>
       </c>
-      <c r="D27" t="n">
-        <v>118</v>
-      </c>
-      <c r="E27" t="inlineStr">
+      <c r="D32" t="n">
+        <v>87</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>06:46:40</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>08:29</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>103</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>06:46:40</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>08:29</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>103</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>06:46:40</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>08:41</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>115</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>06:46:40</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>08:43</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>117</v>
+      </c>
+      <c r="E36" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1036,7 +1261,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1054,14 +1279,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:15:23</t>
+          <t>Última actualización: 06:46:40</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 4</t>
+          <t>Total filas: 7</t>
         </is>
       </c>
     </row>
@@ -1120,12 +1345,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>06:57</t>
+          <t>06:56</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1134,7 +1359,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1145,21 +1370,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>05:47:29</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>06:57</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1170,23 +1395,98 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>06:46:40</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>07:15</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>29</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>06:15:23</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>07:16</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="D10" t="n">
         <v>61</v>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>06:46:40</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>07:43</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>57</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>06:46:40</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>08:43</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>117</v>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1203,7 +1503,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1221,14 +1521,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:15:23</t>
+          <t>Última actualización: 06:46:40</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 1</t>
+          <t>Total filas: 3</t>
         </is>
       </c>
     </row>
@@ -1262,23 +1562,73 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>06:46:40</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>07:42</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>56</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>06:15:23</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>07:43</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="D7" t="n">
         <v>88</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>06:46:40</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>08:35</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>109</v>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1274
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:46:40</t>
+          <t>Última actualización: 06:58:58</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 31</t>
+          <t>Total filas: 45</t>
         </is>
       </c>
     </row>
@@ -703,21 +703,21 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>06:59</t>
+          <t>06:58</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -728,21 +728,21 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>06:58</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,21 +753,21 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>06:59</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -778,21 +778,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>07:19</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -803,21 +803,21 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>07:20</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -828,21 +828,21 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:18</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -858,16 +858,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:19</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -878,21 +878,21 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>07:29</t>
+          <t>07:20</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -903,21 +903,21 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>07:35</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -933,16 +933,16 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>07:36</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -953,21 +953,21 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>07:37</t>
+          <t>07:22</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -978,21 +978,21 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>07:43</t>
+          <t>07:29</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1003,21 +1003,21 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>07:55</t>
+          <t>07:34</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1033,16 +1033,16 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>07:35</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,21 +1053,21 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>08:01</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1078,21 +1078,21 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>08:06</t>
+          <t>07:37</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1103,21 +1103,21 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>08:11</t>
+          <t>07:43</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1128,21 +1128,21 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>08:13</t>
+          <t>07:54</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1158,16 +1158,16 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>08:29</t>
+          <t>07:55</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1178,21 +1178,21 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>08:29</t>
+          <t>07:59</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>103</v>
+        <v>61</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1208,16 +1208,16 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>08:41</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>115</v>
+        <v>74</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1228,23 +1228,373 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
+          <t>06:58:58</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>62</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
           <t>06:46:40</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>08:01</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>75</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>06:46:40</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>08:06</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>80</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>06:58:58</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>08:11</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>73</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>06:58:58</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>08:12</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>74</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>06:46:40</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>08:13</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>87</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>06:58:58</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>08:28</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>90</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>06:58:58</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>08:28</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>90</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>06:46:40</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>08:29</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>103</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>06:46:40</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>08:29</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>103</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>06:58:58</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>08:40</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>102</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>06:46:40</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>08:41</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>115</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>06:58:58</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
         <is>
           <t>08:43</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="C48" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D36" t="n">
-        <v>117</v>
-      </c>
-      <c r="E36" t="inlineStr">
+      <c r="D48" t="n">
+        <v>105</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>06:58:58</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>08:52</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>114</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>06:58:58</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>08:53</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>115</v>
+      </c>
+      <c r="E50" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1261,7 +1611,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1279,14 +1629,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:46:40</t>
+          <t>Última actualización: 06:58:58</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 7</t>
+          <t>Total filas: 9</t>
         </is>
       </c>
     </row>
@@ -1395,21 +1745,21 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>06:58</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -1420,12 +1770,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1434,7 +1784,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -1445,21 +1795,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>07:43</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1470,23 +1820,73 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>07:43</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>45</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>06:58:58</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>08:43</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D12" t="n">
-        <v>117</v>
-      </c>
-      <c r="E12" t="inlineStr">
+      <c r="D13" t="n">
+        <v>105</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>06:58:58</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>08:53</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>115</v>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1503,7 +1903,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1521,14 +1921,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:46:40</t>
+          <t>Última actualización: 06:58:58</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 4</t>
         </is>
       </c>
     </row>
@@ -1562,7 +1962,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1576,7 +1976,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -1612,7 +2012,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1626,11 +2026,36 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>06:58:58</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>08:50</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>112</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1275
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:58:58</t>
+          <t>Última actualización: 07:26:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 45</t>
+          <t>Total filas: 51</t>
         </is>
       </c>
     </row>
@@ -978,7 +978,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1028,7 +1028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1067,7 +1067,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1103,7 +1103,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1117,7 +1117,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1167,7 +1167,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1203,7 +1203,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1213,11 +1213,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1228,7 +1228,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1238,11 +1238,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1278,7 +1278,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1303,7 +1303,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1317,7 +1317,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1367,7 +1367,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1388,7 +1388,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1413,7 +1413,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1428,7 +1428,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1438,11 +1438,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1453,7 +1453,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1463,11 +1463,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1503,7 +1503,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1528,7 +1528,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1542,7 +1542,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1553,12 +1553,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>08:52</t>
+          <t>08:51</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1567,7 +1567,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1583,18 +1583,168 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
+          <t>08:52</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>114</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>07:26:49</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
           <t>08:53</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C51" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D50" t="n">
-        <v>115</v>
-      </c>
-      <c r="E50" t="inlineStr">
+      <c r="D51" t="n">
+        <v>87</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>07:26:49</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>08:57</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>91</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>07:26:49</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>09:06</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>100</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>07:26:49</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>09:16</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>110</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>07:26:49</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>111</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>07:26:49</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>09:18</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>112</v>
+      </c>
+      <c r="E56" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1611,7 +1761,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1629,14 +1779,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:58:58</t>
+          <t>Última actualización: 07:26:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 9</t>
+          <t>Total filas: 10</t>
         </is>
       </c>
     </row>
@@ -1820,7 +1970,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1834,7 +1984,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1845,7 +1995,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1859,7 +2009,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1870,7 +2020,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1884,9 +2034,34 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>07:26:49</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>08:57</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>91</v>
+      </c>
+      <c r="E15" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1921,7 +2096,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:58:58</t>
+          <t>Última actualización: 07:26:49</t>
         </is>
       </c>
     </row>
@@ -1962,7 +2137,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1976,7 +2151,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -2012,7 +2187,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2026,7 +2201,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -2037,7 +2212,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2051,7 +2226,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1276
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:26:49</t>
+          <t>Última actualización: 07:51:40</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 51</t>
+          <t>Total filas: 58</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1153,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1167,7 +1167,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1203,7 +1203,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1213,11 +1213,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1238,7 +1238,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1253,7 +1253,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1267,7 +1267,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1278,7 +1278,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1303,7 +1303,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1317,7 +1317,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1367,7 +1367,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1428,7 +1428,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1438,11 +1438,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1453,7 +1453,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1463,11 +1463,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1503,7 +1503,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1528,7 +1528,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1542,7 +1542,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1553,12 +1553,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>08:51</t>
+          <t>08:45</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1567,7 +1567,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1578,12 +1578,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>08:52</t>
+          <t>08:51</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1592,7 +1592,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1603,21 +1603,21 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>08:52</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>87</v>
+        <v>114</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1628,21 +1628,21 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1658,16 +1658,16 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>09:06</t>
+          <t>08:57</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1678,21 +1678,21 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>08:58</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1703,21 +1703,21 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:06</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1733,18 +1733,193 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
+          <t>09:16</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>110</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>07:51:40</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>86</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>07:51:40</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
           <t>09:18</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="C58" t="inlineStr">
         <is>
           <t>15X38_ABASTO</t>
         </is>
       </c>
-      <c r="D56" t="n">
+      <c r="D58" t="n">
+        <v>87</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>07:51:40</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>90</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>07:51:40</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>09:29</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>98</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>07:51:40</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>09:39</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>108</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>07:51:40</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>110</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>07:51:40</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
         <v>112</v>
       </c>
-      <c r="E56" t="inlineStr">
+      <c r="E63" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1761,7 +1936,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1779,14 +1954,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:26:49</t>
+          <t>Última actualización: 07:51:40</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 10</t>
+          <t>Total filas: 11</t>
         </is>
       </c>
     </row>
@@ -1995,7 +2170,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -2009,7 +2184,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -2020,7 +2195,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -2034,7 +2209,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -2062,6 +2237,31 @@
         <v>91</v>
       </c>
       <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>07:51:40</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>08:58</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>67</v>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2078,7 +2278,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2096,14 +2296,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:26:49</t>
+          <t>Última actualización: 07:51:40</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 4</t>
+          <t>Total filas: 5</t>
         </is>
       </c>
     </row>
@@ -2187,7 +2387,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2201,7 +2401,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -2212,7 +2412,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2226,11 +2426,36 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>07:51:40</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>09:20</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>89</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1277
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:51:40</t>
+          <t>Última actualización: 08:14:55</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 58</t>
+          <t>Total filas: 68</t>
         </is>
       </c>
     </row>
@@ -903,7 +903,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -913,11 +913,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -938,11 +938,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1378,21 +1378,21 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>08:28</t>
+          <t>08:14</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1428,12 +1428,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>08:29</t>
+          <t>08:28</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1478,21 +1478,21 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>08:40</t>
+          <t>08:29</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>102</v>
+        <v>15</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1503,12 +1503,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>08:41</t>
+          <t>08:40</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1528,21 +1528,21 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>08:43</t>
+          <t>08:41</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1553,21 +1553,21 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>08:45</t>
+          <t>08:43</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1578,12 +1578,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>08:51</t>
+          <t>08:45</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1592,7 +1592,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1603,12 +1603,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>08:52</t>
+          <t>08:51</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1617,7 +1617,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>114</v>
+        <v>37</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1628,21 +1628,21 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>08:52</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>62</v>
+        <v>114</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,21 +1653,21 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>91</v>
+        <v>39</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1678,12 +1678,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>08:58</t>
+          <t>08:57</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1692,7 +1692,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1708,16 +1708,16 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>09:06</t>
+          <t>08:58</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,21 +1728,21 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>09:04</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1753,21 +1753,21 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:06</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1778,21 +1778,21 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>09:18</t>
+          <t>09:16</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,21 +1803,21 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1828,21 +1828,21 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>09:29</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>98</v>
+        <v>63</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1853,21 +1853,21 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>09:39</t>
+          <t>09:18</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1883,16 +1883,16 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1903,23 +1903,273 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
+          <t>08:14:55</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>09:28</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>74</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
           <t>07:51:40</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr">
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>09:29</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>98</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>08:14:55</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>09:31</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>77</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>08:14:55</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>09:35</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>81</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>08:14:55</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>09:39</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>85</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>08:14:55</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>87</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>08:14:55</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
         <is>
           <t>09:43</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
+      <c r="C69" t="inlineStr">
         <is>
           <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
-      <c r="D63" t="n">
-        <v>112</v>
-      </c>
-      <c r="E63" t="inlineStr">
+      <c r="D69" t="n">
+        <v>89</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>08:14:55</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>09:53</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>99</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>08:14:55</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>09:58</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>104</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>08:14:55</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>10:05</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>111</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>08:14:55</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>10:13</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>119</v>
+      </c>
+      <c r="E73" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1936,7 +2186,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1954,14 +2204,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:51:40</t>
+          <t>Última actualización: 08:14:55</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 11</t>
+          <t>Total filas: 12</t>
         </is>
       </c>
     </row>
@@ -2170,7 +2420,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -2184,7 +2434,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -2195,7 +2445,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -2209,7 +2459,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -2220,7 +2470,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -2234,7 +2484,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>91</v>
+        <v>43</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -2262,6 +2512,31 @@
         <v>67</v>
       </c>
       <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>08:14:55</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>09:58</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>104</v>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2278,7 +2553,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2296,14 +2571,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:51:40</t>
+          <t>Última actualización: 08:14:55</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 5</t>
+          <t>Total filas: 6</t>
         </is>
       </c>
     </row>
@@ -2387,7 +2662,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2401,7 +2676,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -2412,7 +2687,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2426,7 +2701,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -2437,7 +2712,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2451,11 +2726,36 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>08:14:55</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>10:12</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>118</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1278
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:14:55</t>
+          <t>Última actualización: 08:35:17</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 68</t>
+          <t>Total filas: 79</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1203,7 +1203,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1213,11 +1213,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1228,7 +1228,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1238,11 +1238,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1528,7 +1528,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:35:17</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1542,7 +1542,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1578,21 +1578,21 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:35:17</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>08:45</t>
+          <t>08:44</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1603,12 +1603,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>08:51</t>
+          <t>08:45</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1617,7 +1617,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1628,12 +1628,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>08:52</t>
+          <t>08:51</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1642,7 +1642,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>114</v>
+        <v>37</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,21 +1653,21 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>08:52</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>39</v>
+        <v>114</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1678,21 +1678,21 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:35:17</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1703,21 +1703,21 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>08:58</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,21 +1728,21 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:35:17</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>09:04</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1758,16 +1758,16 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>09:06</t>
+          <t>08:57</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1778,21 +1778,21 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>08:35:17</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>08:58</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>110</v>
+        <v>23</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1808,16 +1808,16 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:04</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1828,21 +1828,21 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:35:17</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:05</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1853,21 +1853,21 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:35:17</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>09:18</t>
+          <t>09:06</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1878,12 +1878,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:16</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1892,7 +1892,7 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1908,16 +1908,16 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>09:28</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1928,21 +1928,21 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:35:17</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>09:29</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1953,21 +1953,21 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:35:17</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>09:31</t>
+          <t>09:18</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,21 +1978,21 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:35:17</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>09:35</t>
+          <t>09:18</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,21 +2003,21 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>09:39</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2033,16 +2033,16 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:28</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2053,21 +2053,21 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:35:17</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:29</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2083,16 +2083,16 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>09:53</t>
+          <t>09:31</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2103,21 +2103,21 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:35:17</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>09:58</t>
+          <t>09:33</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>104</v>
+        <v>58</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2133,16 +2133,16 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>10:05</t>
+          <t>09:35</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2153,23 +2153,298 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
+          <t>08:35:17</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>09:39</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>64</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
           <t>08:14:55</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr">
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>87</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>08:35:17</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>67</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>08:35:17</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>68</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>08:35:17</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>09:53</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>78</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>08:14:55</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>09:58</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>104</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>08:35:17</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>09:59</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>84</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>08:14:55</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>10:05</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>111</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>08:35:17</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>10:06</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>91</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>08:35:17</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
         <is>
           <t>10:13</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="C82" t="inlineStr">
         <is>
           <t>17X38_ROMERO</t>
         </is>
       </c>
-      <c r="D73" t="n">
-        <v>119</v>
-      </c>
-      <c r="E73" t="inlineStr">
+      <c r="D82" t="n">
+        <v>98</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>08:35:17</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>10:25</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>110</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>08:35:17</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>10:29</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>114</v>
+      </c>
+      <c r="E84" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2186,7 +2461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2204,14 +2479,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:14:55</t>
+          <t>Última actualización: 08:35:17</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 12</t>
+          <t>Total filas: 15</t>
         </is>
       </c>
     </row>
@@ -2445,21 +2720,21 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:35:17</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>08:44</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -2475,16 +2750,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -2495,21 +2770,21 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:35:17</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>08:58</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -2525,18 +2800,93 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>08:57</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>43</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>08:35:17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>08:58</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>23</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>08:14:55</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>09:58</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D17" t="n">
+      <c r="D19" t="n">
         <v>104</v>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>08:35:17</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>09:59</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>84</v>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2553,7 +2903,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2571,14 +2921,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:14:55</t>
+          <t>Última actualización: 08:35:17</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 6</t>
+          <t>Total filas: 11</t>
         </is>
       </c>
     </row>
@@ -2687,25 +3037,25 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:35:17</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>08:50</t>
+          <t>08:36</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
@@ -2717,45 +3067,170 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>09:20</t>
+          <t>08:50</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>08:35:17</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>08:51</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>16</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>08:14:55</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>09:20</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>66</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>08:35:17</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>46</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>08:14:55</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>10:12</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="D14" t="n">
         <v>118</v>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>08:35:17</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>10:13</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>98</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>08:35:17</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>10:30</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>115</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1279
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:35:17</t>
+          <t>Última actualización: 08:49:06</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 79</t>
+          <t>Total filas: 83</t>
         </is>
       </c>
     </row>
@@ -903,7 +903,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -913,11 +913,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -938,11 +938,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1453,7 +1453,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1463,11 +1463,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1478,7 +1478,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1488,11 +1488,11 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1628,21 +1628,21 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>08:51</t>
+          <t>08:50</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,12 +1653,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>08:52</t>
+          <t>08:51</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1667,7 +1667,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>114</v>
+        <v>37</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1678,12 +1678,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>08:52</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1692,7 +1692,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>18</v>
+        <v>114</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1728,21 +1728,21 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1753,21 +1753,21 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1778,12 +1778,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>08:58</t>
+          <t>08:57</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1792,7 +1792,7 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,21 +1803,21 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>09:04</t>
+          <t>08:58</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1828,12 +1828,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>09:05</t>
+          <t>09:04</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1842,7 +1842,7 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1853,21 +1853,21 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>09:06</t>
+          <t>09:05</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1878,21 +1878,21 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>09:06</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>110</v>
+        <v>17</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1903,21 +1903,21 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:16</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1938,11 +1938,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1953,21 +1953,21 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>09:18</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1992,7 +1992,7 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,21 +2003,21 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:18</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>90</v>
+        <v>29</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2028,21 +2028,21 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>09:28</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2053,12 +2053,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>09:29</t>
+          <t>09:28</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2067,7 +2067,7 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2078,21 +2078,21 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>09:31</t>
+          <t>09:29</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2103,12 +2103,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>09:33</t>
+          <t>09:31</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2117,7 +2117,7 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2133,16 +2133,16 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>09:35</t>
+          <t>09:31</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2158,16 +2158,16 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>09:39</t>
+          <t>09:33</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2183,16 +2183,16 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:35</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2203,21 +2203,21 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:39</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,21 +2228,21 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:41</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,21 +2253,21 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>09:53</t>
+          <t>09:42</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,21 +2278,21 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>09:58</t>
+          <t>09:43</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>104</v>
+        <v>54</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,21 +2303,21 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>09:59</t>
+          <t>09:53</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2333,16 +2333,16 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>10:05</t>
+          <t>09:58</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2353,21 +2353,21 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>10:06</t>
+          <t>09:59</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2378,21 +2378,21 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>10:13</t>
+          <t>10:05</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2403,21 +2403,21 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>10:25</t>
+          <t>10:06</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>110</v>
+        <v>77</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2428,23 +2428,123 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
+          <t>10:13</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>84</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>08:49:06</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>10:25</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>96</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>08:49:06</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
           <t>10:29</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr">
+      <c r="C86" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D84" t="n">
-        <v>114</v>
-      </c>
-      <c r="E84" t="inlineStr">
+      <c r="D86" t="n">
+        <v>100</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>08:49:06</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>10:44</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>115</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>08:49:06</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>10:46</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>15_P INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>117</v>
+      </c>
+      <c r="E88" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2461,7 +2561,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2479,14 +2579,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:35:17</t>
+          <t>Última actualización: 08:49:06</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 15</t>
+          <t>Total filas: 16</t>
         </is>
       </c>
     </row>
@@ -2745,21 +2845,21 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>08:50</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -2770,12 +2870,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -2784,7 +2884,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -2795,21 +2895,21 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -2820,12 +2920,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>08:58</t>
+          <t>08:57</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -2834,7 +2934,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -2845,21 +2945,21 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>09:58</t>
+          <t>08:58</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>104</v>
+        <v>9</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -2870,23 +2970,48 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>09:58</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>104</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>08:49:06</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>09:59</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D20" t="n">
-        <v>84</v>
-      </c>
-      <c r="E20" t="inlineStr">
+      <c r="D21" t="n">
+        <v>70</v>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2903,7 +3028,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2921,14 +3046,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:35:17</t>
+          <t>Última actualización: 08:49:06</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 11</t>
+          <t>Total filas: 13</t>
         </is>
       </c>
     </row>
@@ -3112,37 +3237,37 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>09:20</t>
+          <t>08:52</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:20</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -3151,7 +3276,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -3162,37 +3287,37 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>10:12</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>118</v>
+        <v>32</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>10:13</t>
+          <t>10:12</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -3201,7 +3326,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -3212,23 +3337,73 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>10:13</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>84</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>08:49:06</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>10:30</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
-      <c r="D16" t="n">
-        <v>115</v>
-      </c>
-      <c r="E16" t="inlineStr">
+      <c r="D17" t="n">
+        <v>101</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>08:49:06</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>10:31</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>102</v>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1280
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:49:06</t>
+          <t>Última actualización: 08:57:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 83</t>
+          <t>Total filas: 85</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1803,7 +1803,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1817,7 +1817,7 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1853,7 +1853,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1867,7 +1867,7 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1878,7 +1878,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1892,7 +1892,7 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1903,7 +1903,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1917,7 +1917,7 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>110</v>
+        <v>19</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1942,7 +1942,7 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2103,7 +2103,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2113,11 +2113,11 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2203,21 +2203,21 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>09:39</t>
+          <t>09:36</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,21 +2228,21 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:39</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,12 +2253,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:41</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2267,7 +2267,7 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2283,16 +2283,16 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:42</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,21 +2303,21 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>09:53</t>
+          <t>09:43</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2328,21 +2328,21 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>09:58</t>
+          <t>09:53</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>104</v>
+        <v>56</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2353,12 +2353,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>09:59</t>
+          <t>09:58</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2367,7 +2367,7 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2378,21 +2378,21 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>10:05</t>
+          <t>09:59</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2403,12 +2403,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>10:06</t>
+          <t>10:05</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2417,7 +2417,7 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2433,16 +2433,16 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>10:13</t>
+          <t>10:06</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2453,21 +2453,21 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>10:25</t>
+          <t>10:13</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,21 +2478,21 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>10:29</t>
+          <t>10:24</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2503,21 +2503,21 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>10:44</t>
+          <t>10:25</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2528,23 +2528,73 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
+          <t>10:29</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>92</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>08:57:42</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>10:44</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>107</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>08:57:42</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
           <t>10:46</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr">
+      <c r="C90" t="inlineStr">
         <is>
           <t>15_P INDUSTRIAL</t>
         </is>
       </c>
-      <c r="D88" t="n">
-        <v>117</v>
-      </c>
-      <c r="E88" t="inlineStr">
+      <c r="D90" t="n">
+        <v>109</v>
+      </c>
+      <c r="E90" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2579,7 +2629,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:49:06</t>
+          <t>Última actualización: 08:57:42</t>
         </is>
       </c>
     </row>
@@ -2945,7 +2995,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2959,7 +3009,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -2970,7 +3020,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2984,7 +3034,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -3028,7 +3078,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3046,14 +3096,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:49:06</t>
+          <t>Última actualización: 08:57:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 13</t>
+          <t>Total filas: 16</t>
         </is>
       </c>
     </row>
@@ -3262,37 +3312,37 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>09:20</t>
+          <t>08:59</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:20</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -3301,7 +3351,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -3312,37 +3362,37 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>10:12</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>118</v>
+        <v>32</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>10:13</t>
+          <t>10:12</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -3351,7 +3401,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -3367,43 +3417,118 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>10:30</t>
+          <t>10:13</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>08:57:42</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>10:29</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>92</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>08:57:42</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>10:30</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>93</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
           <t>08:49:06</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>10:30</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>101</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>08:49:06</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
         <is>
           <t>10:31</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D18" t="n">
+      <c r="D21" t="n">
         <v>102</v>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1281
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:57:42</t>
+          <t>Última actualización: 09:42:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 85</t>
+          <t>Total filas: 97</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1203,7 +1203,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1213,11 +1213,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1228,7 +1228,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1238,11 +1238,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1938,11 +1938,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2103,7 +2103,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2113,11 +2113,11 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2292,7 +2292,7 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2317,7 +2317,7 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2342,7 +2342,7 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2353,21 +2353,21 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>09:58</t>
+          <t>09:55</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2378,12 +2378,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>09:59</t>
+          <t>09:58</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2392,7 +2392,7 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2403,21 +2403,21 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>10:05</t>
+          <t>09:59</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2428,12 +2428,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>10:06</t>
+          <t>10:05</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2442,7 +2442,7 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2453,21 +2453,21 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>10:13</t>
+          <t>10:06</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,21 +2478,21 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>10:24</t>
+          <t>10:13</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>87</v>
+        <v>31</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2503,21 +2503,21 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>10:25</t>
+          <t>10:21</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2533,16 +2533,16 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>10:29</t>
+          <t>10:24</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,21 +2553,21 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>10:44</t>
+          <t>10:25</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>107</v>
+        <v>43</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2578,23 +2578,323 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
+          <t>10:29</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>47</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>09:42:42</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>10:29</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>47</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>09:42:42</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>10:44</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>62</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>09:42:42</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
           <t>10:46</t>
         </is>
       </c>
-      <c r="C90" t="inlineStr">
+      <c r="C93" t="inlineStr">
         <is>
           <t>15_P INDUSTRIAL</t>
         </is>
       </c>
-      <c r="D90" t="n">
-        <v>109</v>
-      </c>
-      <c r="E90" t="inlineStr">
+      <c r="D93" t="n">
+        <v>64</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>09:42:42</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>10:53</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>71</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>09:42:42</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>10:59</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>77</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>09:42:42</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>79</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>09:42:42</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>11:06</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>84</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>09:42:42</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>11:10</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>88</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>09:42:42</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>11:14</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>92</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>09:42:42</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>11:15</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>93</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>09:42:42</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>11:29</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>107</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>09:42:42</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>108</v>
+      </c>
+      <c r="E102" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2611,7 +2911,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2629,14 +2929,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:57:42</t>
+          <t>Última actualización: 09:42:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 16</t>
+          <t>Total filas: 17</t>
         </is>
       </c>
     </row>
@@ -3020,7 +3320,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -3034,7 +3334,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -3062,6 +3362,31 @@
         <v>70</v>
       </c>
       <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>09:42:42</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>108</v>
+      </c>
+      <c r="E22" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3078,7 +3403,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3096,14 +3421,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:57:42</t>
+          <t>Última actualización: 09:42:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 16</t>
+          <t>Total filas: 17</t>
         </is>
       </c>
     </row>
@@ -3387,7 +3712,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -3401,7 +3726,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -3437,7 +3762,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -3451,7 +3776,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>92</v>
+        <v>47</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -3462,7 +3787,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -3472,11 +3797,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -3487,7 +3812,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -3497,11 +3822,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>101</v>
+        <v>48</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -3531,6 +3856,31 @@
       <c r="E21" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>09:42:42</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11:25</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>103</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1282
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:42:42</t>
+          <t>Última actualización: 10:32:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 97</t>
+          <t>Total filas: 111</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -903,7 +903,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -913,11 +913,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -938,11 +938,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1203,7 +1203,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1213,11 +1213,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1228,7 +1228,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1238,11 +1238,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,7 +1428,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1438,11 +1438,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1453,7 +1453,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1463,11 +1463,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1478,7 +1478,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1488,11 +1488,11 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2103,7 +2103,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2113,11 +2113,11 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D90" t="n">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D91" t="n">
@@ -2628,7 +2628,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>09:42:42</t>
+          <t>10:32:07</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -2642,7 +2642,7 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2653,7 +2653,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>09:42:42</t>
+          <t>10:32:07</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -2667,7 +2667,7 @@
         </is>
       </c>
       <c r="D93" t="n">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2703,21 +2703,21 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>09:42:42</t>
+          <t>10:32:07</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>10:59</t>
+          <t>10:55</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2728,21 +2728,21 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>09:42:42</t>
+          <t>10:32:07</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>11:01</t>
+          <t>10:57</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2753,21 +2753,21 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>09:42:42</t>
+          <t>10:32:07</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>11:06</t>
+          <t>10:59</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2778,21 +2778,21 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>09:42:42</t>
+          <t>10:32:07</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>11:10</t>
+          <t>11:01</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2803,21 +2803,21 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>09:42:42</t>
+          <t>10:32:07</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>11:14</t>
+          <t>11:06</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>92</v>
+        <v>34</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,21 +2828,21 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>09:42:42</t>
+          <t>10:32:07</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>11:10</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>93</v>
+        <v>38</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2858,16 +2858,16 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>11:29</t>
+          <t>11:14</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2878,23 +2878,373 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
+          <t>10:32:07</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>11:15</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>43</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>10:32:07</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>11:15</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>43</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>10:32:07</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>11:24</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>52</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>10:32:07</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>11:29</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>57</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
           <t>09:42:42</t>
         </is>
       </c>
-      <c r="B102" t="inlineStr">
+      <c r="B106" t="inlineStr">
         <is>
           <t>11:30</t>
         </is>
       </c>
-      <c r="C102" t="inlineStr">
+      <c r="C106" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D102" t="n">
+      <c r="D106" t="n">
         <v>108</v>
       </c>
-      <c r="E102" t="inlineStr">
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>10:32:07</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>11:31</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>59</v>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>10:32:07</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>11:42</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>70</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>10:32:07</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>11:45</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>73</v>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>10:32:07</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>11:51</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>79</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>10:32:07</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>11:53</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>81</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>10:32:07</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>11:58</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>86</v>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>10:32:07</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>94</v>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>10:32:07</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>12:10</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>98</v>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>10:32:07</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>12:10</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>98</v>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>10:32:07</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>12:22</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>110</v>
+      </c>
+      <c r="E116" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2911,7 +3261,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2929,14 +3279,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:42:42</t>
+          <t>Última actualización: 10:32:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 17</t>
+          <t>Total filas: 20</t>
         </is>
       </c>
     </row>
@@ -3387,6 +3737,81 @@
         <v>108</v>
       </c>
       <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>10:32:07</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>11:31</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>59</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>10:32:07</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>11:42</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>70</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>10:32:07</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>12:22</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>110</v>
+      </c>
+      <c r="E25" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3403,7 +3828,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3421,14 +3846,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:42:42</t>
+          <t>Última actualización: 10:32:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 17</t>
+          <t>Total filas: 20</t>
         </is>
       </c>
     </row>
@@ -3787,7 +4212,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -3797,11 +4222,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>101</v>
+        <v>48</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -3812,7 +4237,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>09:42:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -3822,11 +4247,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -3862,23 +4287,98 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>10:32:07</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>10:32</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>10:32:07</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>10:32</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
           <t>09:42:42</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B24" t="inlineStr">
         <is>
           <t>11:25</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D22" t="n">
+      <c r="D24" t="n">
         <v>103</v>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>10:32:07</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>11:26</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>54</v>
+      </c>
+      <c r="E25" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1283
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:E126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:32:07</t>
+          <t>Última actualización: 11:01:19</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 111</t>
+          <t>Total filas: 121</t>
         </is>
       </c>
     </row>
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2103,7 +2103,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2113,11 +2113,11 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D90" t="n">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D91" t="n">
@@ -2803,21 +2803,21 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>11:06</t>
+          <t>11:02</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2828,21 +2828,21 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>11:10</t>
+          <t>11:06</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2853,21 +2853,21 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>09:42:42</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>11:14</t>
+          <t>11:10</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>92</v>
+        <v>9</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2878,21 +2878,21 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>11:14</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2928,21 +2928,21 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>11:24</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -2958,16 +2958,16 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>11:29</t>
+          <t>11:24</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2978,21 +2978,21 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>09:42:42</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>11:30</t>
+          <t>11:25</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>108</v>
+        <v>24</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3003,21 +3003,21 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>11:31</t>
+          <t>11:29</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3028,21 +3028,21 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>11:42</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3053,21 +3053,21 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>11:45</t>
+          <t>11:31</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3078,21 +3078,21 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>11:51</t>
+          <t>11:41</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3108,16 +3108,16 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>11:53</t>
+          <t>11:42</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3128,21 +3128,21 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:45</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,21 +3153,21 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>11:47</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>94</v>
+        <v>46</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3183,16 +3183,16 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>11:51</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3203,21 +3203,21 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>11:53</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3228,23 +3228,273 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
+          <t>11:01:19</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>11:58</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>57</v>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>11:01:19</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>12:05</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>64</v>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
           <t>10:32:07</t>
         </is>
       </c>
-      <c r="B116" t="inlineStr">
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>94</v>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>11:01:19</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>12:10</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>69</v>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>11:01:19</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>12:10</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>69</v>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>11:01:19</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>12:17</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>76</v>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>11:01:19</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
         <is>
           <t>12:22</t>
         </is>
       </c>
-      <c r="C116" t="inlineStr">
+      <c r="C122" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D116" t="n">
-        <v>110</v>
-      </c>
-      <c r="E116" t="inlineStr">
+      <c r="D122" t="n">
+        <v>81</v>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>11:01:19</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>12:32</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D123" t="n">
+        <v>91</v>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>11:01:19</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>12:34</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>93</v>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>11:01:19</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>12:37</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D125" t="n">
+        <v>96</v>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>11:01:19</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D126" t="n">
+        <v>107</v>
+      </c>
+      <c r="E126" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3261,7 +3511,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3279,14 +3529,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:32:07</t>
+          <t>Última actualización: 11:01:19</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 20</t>
+          <t>Total filas: 21</t>
         </is>
       </c>
     </row>
@@ -3745,7 +3995,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -3759,7 +4009,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -3770,12 +4020,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>11:42</t>
+          <t>11:41</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -3784,7 +4034,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -3800,18 +4050,43 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
+          <t>11:42</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>70</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>11:01:19</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
           <t>12:22</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D25" t="n">
-        <v>110</v>
-      </c>
-      <c r="E25" t="inlineStr">
+      <c r="D26" t="n">
+        <v>81</v>
+      </c>
+      <c r="E26" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3846,7 +4121,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:32:07</t>
+          <t>Última actualización: 11:01:19</t>
         </is>
       </c>
     </row>
@@ -4362,7 +4637,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -4376,7 +4651,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1284
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E126"/>
+  <dimension ref="A1:E137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:01:19</t>
+          <t>Última actualización: 11:38:09</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 121</t>
+          <t>Total filas: 132</t>
         </is>
       </c>
     </row>
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2103,7 +2103,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2113,11 +2113,11 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>10:32:07</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3103,7 +3103,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3117,7 +3117,7 @@
         </is>
       </c>
       <c r="D111" t="n">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3142,7 +3142,7 @@
         </is>
       </c>
       <c r="D112" t="n">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3203,21 +3203,21 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>11:53</t>
+          <t>11:52</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3228,21 +3228,21 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:53</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3253,21 +3253,21 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>12:05</t>
+          <t>11:58</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3278,12 +3278,12 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>12:05</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -3292,7 +3292,7 @@
         </is>
       </c>
       <c r="D118" t="n">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3303,21 +3303,21 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3328,7 +3328,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -3338,11 +3338,11 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3353,21 +3353,21 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>12:17</t>
+          <t>12:10</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -3378,21 +3378,21 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>12:22</t>
+          <t>12:17</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3403,21 +3403,21 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>12:32</t>
+          <t>12:22</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>91</v>
+        <v>44</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3428,21 +3428,21 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>12:34</t>
+          <t>12:27</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3453,21 +3453,21 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>12:37</t>
+          <t>12:31</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3483,18 +3483,293 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
+          <t>12:32</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D126" t="n">
+        <v>91</v>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>11:38:09</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>12:33</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>55</v>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>11:38:09</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>12:34</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>56</v>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>11:38:09</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>12:37</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D129" t="n">
+        <v>59</v>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>11:38:09</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
           <t>12:48</t>
         </is>
       </c>
-      <c r="C126" t="inlineStr">
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>70</v>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>11:38:09</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
         <is>
           <t>16_SANTA ANA</t>
         </is>
       </c>
-      <c r="D126" t="n">
+      <c r="D131" t="n">
+        <v>70</v>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>11:38:09</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>13:03</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>85</v>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>11:38:09</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>86</v>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>11:38:09</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>95</v>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>11:38:09</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>13:17</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>99</v>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>11:38:09</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>13:25</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D136" t="n">
         <v>107</v>
       </c>
-      <c r="E126" t="inlineStr">
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>11:38:09</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>13:33</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>115</v>
+      </c>
+      <c r="E137" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3511,7 +3786,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3529,14 +3804,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:01:19</t>
+          <t>Última actualización: 11:38:09</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 21</t>
+          <t>Total filas: 23</t>
         </is>
       </c>
     </row>
@@ -4045,7 +4320,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -4059,7 +4334,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -4070,7 +4345,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -4084,9 +4359,59 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>11:38:09</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>86</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>11:38:09</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13:33</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>115</v>
+      </c>
+      <c r="E28" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4103,7 +4428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4121,14 +4446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:01:19</t>
+          <t>Última actualización: 11:38:09</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 20</t>
+          <t>Total filas: 22</t>
         </is>
       </c>
     </row>
@@ -4487,7 +4812,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>09:42:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -4497,11 +4822,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -4512,7 +4837,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -4522,11 +4847,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>101</v>
+        <v>48</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -4656,6 +4981,56 @@
       <c r="E25" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>11:38:09</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>13:12</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>94</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>11:38:09</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>103</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1285
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E137"/>
+  <dimension ref="A1:E147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:38:09</t>
+          <t>Última actualización: 11:56:32</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 132</t>
+          <t>Total filas: 142</t>
         </is>
       </c>
     </row>
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2103,7 +2103,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2113,11 +2113,11 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D90" t="n">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D91" t="n">
@@ -3253,21 +3253,21 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:56</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3278,21 +3278,21 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>12:05</t>
+          <t>11:56</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3308,16 +3308,16 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>11:58</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3328,21 +3328,21 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>12:05</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3358,16 +3358,16 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -3383,16 +3383,16 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>12:17</t>
+          <t>12:10</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3403,21 +3403,21 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>12:22</t>
+          <t>12:10</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3428,21 +3428,21 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>12:27</t>
+          <t>12:17</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3453,21 +3453,21 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>12:31</t>
+          <t>12:22</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3478,12 +3478,12 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>12:32</t>
+          <t>12:27</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -3492,7 +3492,7 @@
         </is>
       </c>
       <c r="D126" t="n">
-        <v>91</v>
+        <v>49</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3508,16 +3508,16 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>12:33</t>
+          <t>12:31</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3528,21 +3528,21 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>12:34</t>
+          <t>12:32</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3558,16 +3558,16 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>12:37</t>
+          <t>12:33</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3578,21 +3578,21 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:34</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3603,21 +3603,21 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3628,21 +3628,21 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3658,16 +3658,16 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>13:04</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,12 +3678,12 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>13:13</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -3692,7 +3692,7 @@
         </is>
       </c>
       <c r="D134" t="n">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,21 +3703,21 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>13:17</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>99</v>
+        <v>52</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3728,21 +3728,21 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>13:25</t>
+          <t>13:02</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3758,18 +3758,268 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
+          <t>13:03</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>85</v>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>11:56:32</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
+        <v>68</v>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>11:38:09</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D139" t="n">
+        <v>95</v>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>11:56:32</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>13:17</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D140" t="n">
+        <v>81</v>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>11:56:32</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>13:24</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>88</v>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>11:56:32</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>13:25</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D142" t="n">
+        <v>89</v>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>11:56:32</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>13:32</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D143" t="n">
+        <v>96</v>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>11:56:32</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
           <t>13:33</t>
         </is>
       </c>
-      <c r="C137" t="inlineStr">
+      <c r="C144" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D137" t="n">
-        <v>115</v>
-      </c>
-      <c r="E137" t="inlineStr">
+      <c r="D144" t="n">
+        <v>97</v>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>11:56:32</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>13:47</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D145" t="n">
+        <v>111</v>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>11:56:32</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>13:52</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D146" t="n">
+        <v>116</v>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>11:56:32</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>13:54</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D147" t="n">
+        <v>118</v>
+      </c>
+      <c r="E147" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3804,7 +4054,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:38:09</t>
+          <t>Última actualización: 11:56:32</t>
         </is>
       </c>
     </row>
@@ -4345,7 +4595,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -4359,7 +4609,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -4370,7 +4620,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -4384,7 +4634,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -4395,7 +4645,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -4409,7 +4659,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -4446,7 +4696,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:38:09</t>
+          <t>Última actualización: 11:56:32</t>
         </is>
       </c>
     </row>
@@ -4987,7 +5237,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -5001,7 +5251,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -5012,7 +5262,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -5026,7 +5276,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1286
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E147"/>
+  <dimension ref="A1:E152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:56:32</t>
+          <t>Última actualización: 12:18:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 142</t>
+          <t>Total filas: 147</t>
         </is>
       </c>
     </row>
@@ -903,7 +903,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -913,11 +913,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -938,11 +938,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,7 +1428,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1438,11 +1438,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1453,7 +1453,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1463,11 +1463,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1478,7 +1478,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1488,11 +1488,11 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2103,7 +2103,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2113,11 +2113,11 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3263,7 +3263,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D117" t="n">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3453,12 +3453,12 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>12:22</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -3467,7 +3467,7 @@
         </is>
       </c>
       <c r="D125" t="n">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3478,21 +3478,21 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>12:27</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3503,21 +3503,21 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>12:31</t>
+          <t>12:22</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3528,12 +3528,12 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>12:32</t>
+          <t>12:27</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -3542,7 +3542,7 @@
         </is>
       </c>
       <c r="D128" t="n">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3558,16 +3558,16 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>12:33</t>
+          <t>12:31</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3578,21 +3578,21 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>12:34</t>
+          <t>12:32</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3603,21 +3603,21 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:33</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3628,21 +3628,21 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:34</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,21 +3653,21 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>12:37</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,21 +3678,21 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,21 +3703,21 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3728,21 +3728,21 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>13:02</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3753,21 +3753,21 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3778,21 +3778,21 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>13:04</t>
+          <t>13:02</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3803,21 +3803,21 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>13:13</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D139" t="n">
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -3828,21 +3828,21 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>13:17</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3858,16 +3858,16 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>13:24</t>
+          <t>13:04</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -3878,21 +3878,21 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>13:25</t>
+          <t>13:13</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3903,21 +3903,21 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>13:32</t>
+          <t>13:17</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3933,16 +3933,16 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>13:33</t>
+          <t>13:24</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -3953,21 +3953,21 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>13:47</t>
+          <t>13:25</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D145" t="n">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -3978,21 +3978,21 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>13:52</t>
+          <t>13:25</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4003,23 +4003,148 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
+          <t>12:18:38</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>13:32</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D147" t="n">
+        <v>74</v>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>12:18:38</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>13:33</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D148" t="n">
+        <v>75</v>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>12:18:38</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>13:47</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D149" t="n">
+        <v>89</v>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
           <t>11:56:32</t>
         </is>
       </c>
-      <c r="B147" t="inlineStr">
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>13:52</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D150" t="n">
+        <v>116</v>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>12:18:38</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
         <is>
           <t>13:54</t>
         </is>
       </c>
-      <c r="C147" t="inlineStr">
+      <c r="C151" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D147" t="n">
+      <c r="D151" t="n">
+        <v>96</v>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>12:18:38</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>14:16</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D152" t="n">
         <v>118</v>
       </c>
-      <c r="E147" t="inlineStr">
+      <c r="E152" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4036,7 +4161,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4054,14 +4179,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:56:32</t>
+          <t>Última actualización: 12:18:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 23</t>
+          <t>Total filas: 25</t>
         </is>
       </c>
     </row>
@@ -4595,12 +4720,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>12:22</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -4609,7 +4734,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -4625,7 +4750,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>13:04</t>
+          <t>12:22</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -4634,7 +4759,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -4645,23 +4770,73 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>12:18:38</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13:03</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>45</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
           <t>11:56:32</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>68</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>12:18:38</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
         <is>
           <t>13:33</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D28" t="n">
-        <v>97</v>
-      </c>
-      <c r="E28" t="inlineStr">
+      <c r="D30" t="n">
+        <v>75</v>
+      </c>
+      <c r="E30" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4678,7 +4853,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4696,14 +4871,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:56:32</t>
+          <t>Última actualización: 12:18:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 22</t>
+          <t>Total filas: 25</t>
         </is>
       </c>
     </row>
@@ -5237,12 +5412,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>13:12</t>
+          <t>13:11</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -5251,7 +5426,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -5267,20 +5442,95 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>13:12</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>76</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>12:18:38</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13:20</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>62</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>11:56:32</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
           <t>13:21</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
-      <c r="D27" t="n">
+      <c r="D29" t="n">
         <v>85</v>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>12:18:38</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>98</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1287
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E152"/>
+  <dimension ref="A1:E163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:18:38</t>
+          <t>Última actualización: 12:43:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 147</t>
+          <t>Total filas: 158</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -903,7 +903,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -913,11 +913,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -938,11 +938,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1938,11 +1938,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -3263,7 +3263,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D117" t="n">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3463,7 +3463,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D125" t="n">
@@ -3488,7 +3488,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D126" t="n">
@@ -3728,7 +3728,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -3742,7 +3742,7 @@
         </is>
       </c>
       <c r="D136" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3753,7 +3753,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -3763,11 +3763,11 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3783,16 +3783,16 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>13:02</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3808,16 +3808,16 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>13:02</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D139" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -3828,7 +3828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3838,11 +3838,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,21 +3853,21 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>13:04</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -3878,21 +3878,21 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>13:13</t>
+          <t>13:04</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3903,21 +3903,21 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>13:17</t>
+          <t>13:13</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3928,21 +3928,21 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>13:24</t>
+          <t>13:17</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -3953,21 +3953,21 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>13:25</t>
+          <t>13:19</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D145" t="n">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -3978,12 +3978,12 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>13:25</t>
+          <t>13:24</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -3992,7 +3992,7 @@
         </is>
       </c>
       <c r="D146" t="n">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4003,21 +4003,21 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>13:32</t>
+          <t>13:25</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,21 +4028,21 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>13:33</t>
+          <t>13:25</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4058,16 +4058,16 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>13:47</t>
+          <t>13:32</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4078,21 +4078,21 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>13:52</t>
+          <t>13:33</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D150" t="n">
-        <v>116</v>
+        <v>50</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -4103,21 +4103,21 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>13:54</t>
+          <t>13:33</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>96</v>
+        <v>50</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,23 +4128,298 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
+          <t>12:43:13</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>13:47</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D152" t="n">
+        <v>64</v>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>11:56:32</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>13:52</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D153" t="n">
+        <v>116</v>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>12:43:13</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>13:54</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D154" t="n">
+        <v>71</v>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>12:43:13</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>14:02</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D155" t="n">
+        <v>79</v>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>12:43:13</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>14:05</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D156" t="n">
+        <v>82</v>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
           <t>12:18:38</t>
         </is>
       </c>
-      <c r="B152" t="inlineStr">
+      <c r="B157" t="inlineStr">
         <is>
           <t>14:16</t>
         </is>
       </c>
-      <c r="C152" t="inlineStr">
+      <c r="C157" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="D152" t="n">
+      <c r="D157" t="n">
         <v>118</v>
       </c>
-      <c r="E152" t="inlineStr">
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>12:43:13</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>14:17</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D158" t="n">
+        <v>94</v>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>12:43:13</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>14:18</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D159" t="n">
+        <v>95</v>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>12:43:13</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>14:27</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D160" t="n">
+        <v>104</v>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>12:43:13</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>14:32</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D161" t="n">
+        <v>109</v>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>12:43:13</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D162" t="n">
+        <v>111</v>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>12:43:13</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>14:39</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D163" t="n">
+        <v>116</v>
+      </c>
+      <c r="E163" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4161,7 +4436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4179,14 +4454,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:18:38</t>
+          <t>Última actualización: 12:43:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 25</t>
+          <t>Total filas: 26</t>
         </is>
       </c>
     </row>
@@ -4795,7 +5070,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -4809,7 +5084,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -4820,7 +5095,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -4834,9 +5109,34 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>12:43:13</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>111</v>
+      </c>
+      <c r="E31" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4853,7 +5153,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4871,14 +5171,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:18:38</t>
+          <t>Última actualización: 12:43:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 25</t>
+          <t>Total filas: 26</t>
         </is>
       </c>
     </row>
@@ -5322,7 +5622,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -5347,7 +5647,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -5437,7 +5737,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -5451,7 +5751,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -5487,7 +5787,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -5501,7 +5801,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>85</v>
+        <v>38</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -5529,6 +5829,31 @@
         <v>98</v>
       </c>
       <c r="E30" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>12:43:13</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>13:57</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>74</v>
+      </c>
+      <c r="E31" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1288
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E163"/>
+  <dimension ref="A1:E168"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:43:13</t>
+          <t>Última actualización: 12:58:23</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 158</t>
+          <t>Total filas: 163</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1453,7 +1453,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1463,11 +1463,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1478,7 +1478,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1488,11 +1488,11 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2103,7 +2103,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2113,11 +2113,11 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3728,7 +3728,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -3738,11 +3738,11 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3778,7 +3778,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3788,11 +3788,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3803,7 +3803,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -3817,7 +3817,7 @@
         </is>
       </c>
       <c r="D139" t="n">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -3828,7 +3828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3838,11 +3838,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3863,11 +3863,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -3878,7 +3878,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3892,7 +3892,7 @@
         </is>
       </c>
       <c r="D142" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3903,7 +3903,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -3917,7 +3917,7 @@
         </is>
       </c>
       <c r="D143" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3928,7 +3928,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -3942,7 +3942,7 @@
         </is>
       </c>
       <c r="D144" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -3953,7 +3953,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -3967,7 +3967,7 @@
         </is>
       </c>
       <c r="D145" t="n">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -3978,12 +3978,12 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>13:24</t>
+          <t>13:23</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -3992,7 +3992,7 @@
         </is>
       </c>
       <c r="D146" t="n">
-        <v>88</v>
+        <v>25</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4003,21 +4003,21 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>13:25</t>
+          <t>13:24</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4053,21 +4053,21 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>13:32</t>
+          <t>13:25</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4078,21 +4078,21 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>13:33</t>
+          <t>13:32</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D150" t="n">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4133,16 +4133,16 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>13:47</t>
+          <t>13:33</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,21 +4153,21 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>13:52</t>
+          <t>13:47</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4178,21 +4178,21 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>13:54</t>
+          <t>13:52</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4203,21 +4203,21 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>14:02</t>
+          <t>13:54</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D155" t="n">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -4228,21 +4228,21 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>14:05</t>
+          <t>14:02</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4253,21 +4253,21 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>14:16</t>
+          <t>14:04</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D157" t="n">
-        <v>118</v>
+        <v>66</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -4283,16 +4283,16 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:05</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -4303,21 +4303,21 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>14:18</t>
+          <t>14:16</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D159" t="n">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -4328,21 +4328,21 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>14:27</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4353,21 +4353,21 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>14:32</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4383,16 +4383,16 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>14:34</t>
+          <t>14:18</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4403,23 +4403,148 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
+          <t>14:27</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D163" t="n">
+        <v>89</v>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>12:58:23</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>14:32</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D164" t="n">
+        <v>94</v>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>12:58:23</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D165" t="n">
+        <v>96</v>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>12:58:23</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
           <t>14:39</t>
         </is>
       </c>
-      <c r="C163" t="inlineStr">
+      <c r="C166" t="inlineStr">
         <is>
           <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
-      <c r="D163" t="n">
+      <c r="D166" t="n">
+        <v>101</v>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>12:58:23</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>14:47</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D167" t="n">
+        <v>109</v>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>12:58:23</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>14:54</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D168" t="n">
         <v>116</v>
       </c>
-      <c r="E163" t="inlineStr">
+      <c r="E168" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4436,7 +4561,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4454,14 +4579,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:43:13</t>
+          <t>Última actualización: 12:58:23</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 26</t>
+          <t>Total filas: 28</t>
         </is>
       </c>
     </row>
@@ -5070,7 +5195,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -5084,7 +5209,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -5095,7 +5220,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -5109,7 +5234,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -5120,7 +5245,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -5134,9 +5259,59 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>12:58:23</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>14:47</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>109</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>12:58:23</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>14:54</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>116</v>
+      </c>
+      <c r="E33" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5171,7 +5346,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:43:13</t>
+          <t>Última actualización: 12:58:23</t>
         </is>
       </c>
     </row>
@@ -5622,7 +5797,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -5647,7 +5822,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -5737,7 +5912,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -5751,7 +5926,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -5787,7 +5962,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -5801,7 +5976,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -5837,7 +6012,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -5851,7 +6026,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1289
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E168"/>
+  <dimension ref="A1:E175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:58:23</t>
+          <t>Última actualización: 13:28:27</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 163</t>
+          <t>Total filas: 170</t>
         </is>
       </c>
     </row>
@@ -1453,7 +1453,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1463,11 +1463,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1478,7 +1478,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1488,11 +1488,11 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2103,7 +2103,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2113,11 +2113,11 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>10:32:07</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3263,7 +3263,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D117" t="n">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3378,7 +3378,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -3388,11 +3388,11 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3403,7 +3403,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -3413,11 +3413,11 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3763,7 +3763,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D137" t="n">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4053,7 +4053,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -4063,11 +4063,11 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4078,7 +4078,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -4092,7 +4092,7 @@
         </is>
       </c>
       <c r="D150" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4167,7 +4167,7 @@
         </is>
       </c>
       <c r="D153" t="n">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4203,7 +4203,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -4217,7 +4217,7 @@
         </is>
       </c>
       <c r="D155" t="n">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -4228,7 +4228,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -4242,7 +4242,7 @@
         </is>
       </c>
       <c r="D156" t="n">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4303,21 +4303,21 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>14:16</t>
+          <t>14:06</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D159" t="n">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -4328,21 +4328,21 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:14</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4353,21 +4353,21 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:16</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,12 +4378,12 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>14:18</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -4392,7 +4392,7 @@
         </is>
       </c>
       <c r="D162" t="n">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4408,16 +4408,16 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>14:27</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D163" t="n">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -4428,21 +4428,21 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>14:32</t>
+          <t>14:18</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,21 +4453,21 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>14:34</t>
+          <t>14:27</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4478,21 +4478,21 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>14:39</t>
+          <t>14:32</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D166" t="n">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -4503,21 +4503,21 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>14:47</t>
+          <t>14:34</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>109</v>
+        <v>66</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4528,23 +4528,198 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
+          <t>14:39</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D168" t="n">
+        <v>71</v>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>13:28:27</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>14:47</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D169" t="n">
+        <v>79</v>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>13:28:27</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>14:51</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D170" t="n">
+        <v>83</v>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>13:28:27</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>14:51</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D171" t="n">
+        <v>83</v>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>13:28:27</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
           <t>14:54</t>
         </is>
       </c>
-      <c r="C168" t="inlineStr">
+      <c r="C172" t="inlineStr">
         <is>
           <t>215_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D168" t="n">
-        <v>116</v>
-      </c>
-      <c r="E168" t="inlineStr">
+      <c r="D172" t="n">
+        <v>86</v>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>13:28:27</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>15:02</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D173" t="n">
+        <v>94</v>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>13:28:27</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>15:11</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D174" t="n">
+        <v>103</v>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>13:28:27</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>15:13</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D175" t="n">
+        <v>105</v>
+      </c>
+      <c r="E175" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4579,7 +4754,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:58:23</t>
+          <t>Última actualización: 13:28:27</t>
         </is>
       </c>
     </row>
@@ -5220,7 +5395,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -5234,7 +5409,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -5245,7 +5420,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -5259,7 +5434,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -5270,7 +5445,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -5284,7 +5459,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -5295,7 +5470,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -5309,7 +5484,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -5328,7 +5503,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5346,14 +5521,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:58:23</t>
+          <t>Última actualización: 13:28:27</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 26</t>
+          <t>Total filas: 28</t>
         </is>
       </c>
     </row>
@@ -5797,7 +5972,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -5822,7 +5997,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -6012,7 +6187,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -6026,11 +6201,61 @@
         </is>
       </c>
       <c r="D31" t="n">
+        <v>29</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>13:28:27</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>14:27</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
         <v>59</v>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="E32" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>13:28:27</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>15:22</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>114</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1290
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E175"/>
+  <dimension ref="A1:E180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:28:27</t>
+          <t>Última actualización: 13:54:35</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 170</t>
+          <t>Total filas: 175</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -903,7 +903,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -913,11 +913,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -938,11 +938,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1203,7 +1203,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1213,11 +1213,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1228,7 +1228,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1238,11 +1238,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,7 +1428,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1438,11 +1438,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1453,7 +1453,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1463,11 +1463,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1478,7 +1478,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1488,11 +1488,11 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2103,7 +2103,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2113,11 +2113,11 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D90" t="n">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D91" t="n">
@@ -3378,7 +3378,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -3388,11 +3388,11 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3403,7 +3403,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -3413,11 +3413,11 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3763,7 +3763,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D137" t="n">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4203,7 +4203,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -4217,7 +4217,7 @@
         </is>
       </c>
       <c r="D155" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -4228,7 +4228,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -4242,7 +4242,7 @@
         </is>
       </c>
       <c r="D156" t="n">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4303,7 +4303,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -4317,7 +4317,7 @@
         </is>
       </c>
       <c r="D159" t="n">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -4328,7 +4328,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4342,7 +4342,7 @@
         </is>
       </c>
       <c r="D160" t="n">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4367,7 +4367,7 @@
         </is>
       </c>
       <c r="D161" t="n">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4392,7 +4392,7 @@
         </is>
       </c>
       <c r="D162" t="n">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4453,7 +4453,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -4467,7 +4467,7 @@
         </is>
       </c>
       <c r="D165" t="n">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4478,7 +4478,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -4492,7 +4492,7 @@
         </is>
       </c>
       <c r="D166" t="n">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -4503,7 +4503,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -4517,7 +4517,7 @@
         </is>
       </c>
       <c r="D167" t="n">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4528,7 +4528,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -4542,7 +4542,7 @@
         </is>
       </c>
       <c r="D168" t="n">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -4567,7 +4567,7 @@
         </is>
       </c>
       <c r="D169" t="n">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4578,7 +4578,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -4588,11 +4588,11 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4603,7 +4603,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -4613,11 +4613,11 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4628,7 +4628,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -4642,7 +4642,7 @@
         </is>
       </c>
       <c r="D172" t="n">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4653,7 +4653,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -4667,7 +4667,7 @@
         </is>
       </c>
       <c r="D173" t="n">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4703,7 +4703,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4717,9 +4717,134 @@
         </is>
       </c>
       <c r="D175" t="n">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="E175" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>13:54:35</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>15:17</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D176" t="n">
+        <v>83</v>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>13:54:35</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D177" t="n">
+        <v>100</v>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>13:54:35</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>15:41</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D178" t="n">
+        <v>107</v>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>13:54:35</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D179" t="n">
+        <v>119</v>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>13:54:35</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D180" t="n">
+        <v>119</v>
+      </c>
+      <c r="E180" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4736,7 +4861,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4754,14 +4879,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:28:27</t>
+          <t>Última actualización: 13:54:35</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 28</t>
+          <t>Total filas: 29</t>
         </is>
       </c>
     </row>
@@ -5420,7 +5545,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -5434,7 +5559,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -5445,7 +5570,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -5459,7 +5584,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -5470,7 +5595,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -5484,9 +5609,34 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>13:54:35</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>100</v>
+      </c>
+      <c r="E34" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5503,7 +5653,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5521,14 +5671,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:28:27</t>
+          <t>Última actualización: 13:54:35</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 28</t>
+          <t>Total filas: 29</t>
         </is>
       </c>
     </row>
@@ -5887,7 +6037,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -5897,11 +6047,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>101</v>
+        <v>48</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -5912,7 +6062,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>09:42:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -5922,11 +6072,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -6162,7 +6312,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -6176,7 +6326,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>98</v>
+        <v>2</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -6212,12 +6362,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>14:27</t>
+          <t>14:26</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -6226,7 +6376,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -6242,18 +6392,43 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
+          <t>14:27</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>59</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>13:54:35</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
           <t>15:22</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D33" t="n">
-        <v>114</v>
-      </c>
-      <c r="E33" t="inlineStr">
+      <c r="D34" t="n">
+        <v>88</v>
+      </c>
+      <c r="E34" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1291
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E180"/>
+  <dimension ref="A1:E188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:54:35</t>
+          <t>Última actualización: 14:17:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 175</t>
+          <t>Total filas: 183</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -903,7 +903,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -913,11 +913,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -938,11 +938,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,7 +1428,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1438,11 +1438,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1453,7 +1453,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1463,11 +1463,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1478,7 +1478,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1488,11 +1488,11 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1938,11 +1938,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -3263,7 +3263,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D117" t="n">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3378,7 +3378,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -3388,11 +3388,11 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3403,7 +3403,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -3413,11 +3413,11 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3763,7 +3763,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D137" t="n">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4053,7 +4053,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -4063,11 +4063,11 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4392,7 +4392,7 @@
         </is>
       </c>
       <c r="D162" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4403,7 +4403,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -4417,7 +4417,7 @@
         </is>
       </c>
       <c r="D163" t="n">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -4453,7 +4453,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -4467,7 +4467,7 @@
         </is>
       </c>
       <c r="D165" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4478,7 +4478,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -4492,7 +4492,7 @@
         </is>
       </c>
       <c r="D166" t="n">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -4503,7 +4503,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -4517,7 +4517,7 @@
         </is>
       </c>
       <c r="D167" t="n">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4528,7 +4528,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -4542,7 +4542,7 @@
         </is>
       </c>
       <c r="D168" t="n">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4578,21 +4578,21 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>14:51</t>
+          <t>14:48</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4603,7 +4603,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -4617,7 +4617,7 @@
         </is>
       </c>
       <c r="D171" t="n">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4628,21 +4628,21 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>14:54</t>
+          <t>14:51</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4653,21 +4653,21 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>15:02</t>
+          <t>14:54</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4678,21 +4678,21 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>15:11</t>
+          <t>15:02</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>103</v>
+        <v>45</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4703,21 +4703,21 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>15:13</t>
+          <t>15:11</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4728,21 +4728,21 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>15:17</t>
+          <t>15:13</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4758,16 +4758,16 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>15:34</t>
+          <t>15:17</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4778,21 +4778,21 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>15:41</t>
+          <t>15:18</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>107</v>
+        <v>61</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4803,21 +4803,21 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:29</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>119</v>
+        <v>72</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4828,23 +4828,223 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
+          <t>14:17:13</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D180" t="n">
+        <v>77</v>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>14:17:13</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>15:36</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D181" t="n">
+        <v>79</v>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
           <t>13:54:35</t>
         </is>
       </c>
-      <c r="B180" t="inlineStr">
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>15:41</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D182" t="n">
+        <v>107</v>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>14:17:13</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>15:42</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D183" t="n">
+        <v>85</v>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>14:17:13</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
         <is>
           <t>15:53</t>
         </is>
       </c>
-      <c r="C180" t="inlineStr">
+      <c r="C184" t="inlineStr">
         <is>
           <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
-      <c r="D180" t="n">
-        <v>119</v>
-      </c>
-      <c r="E180" t="inlineStr">
+      <c r="D184" t="n">
+        <v>96</v>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>14:17:13</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D185" t="n">
+        <v>96</v>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>14:17:13</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>15:57</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D186" t="n">
+        <v>100</v>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>14:17:13</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>16:06</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D187" t="n">
+        <v>109</v>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>14:17:13</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>16:14</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D188" t="n">
+        <v>117</v>
+      </c>
+      <c r="E188" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4861,7 +5061,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4879,14 +5079,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:54:35</t>
+          <t>Última actualización: 14:17:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 29</t>
+          <t>Total filas: 30</t>
         </is>
       </c>
     </row>
@@ -5545,7 +5745,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -5559,7 +5759,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -5595,21 +5795,21 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>14:54</t>
+          <t>14:48</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -5620,23 +5820,48 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
+          <t>14:54</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>37</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>14:17:13</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
           <t>15:34</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C35" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D34" t="n">
-        <v>100</v>
-      </c>
-      <c r="E34" t="inlineStr">
+      <c r="D35" t="n">
+        <v>77</v>
+      </c>
+      <c r="E35" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5653,7 +5878,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5671,14 +5896,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:54:35</t>
+          <t>Última actualización: 14:17:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 29</t>
+          <t>Total filas: 30</t>
         </is>
       </c>
     </row>
@@ -6037,7 +6262,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>09:42:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -6047,11 +6272,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -6062,7 +6287,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -6072,11 +6297,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>101</v>
+        <v>48</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -6387,7 +6612,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -6401,7 +6626,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -6412,7 +6637,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -6426,11 +6651,36 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>14:17:13</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>16:02</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>105</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1292
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E188"/>
+  <dimension ref="A1:E199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:17:13</t>
+          <t>Última actualización: 14:44:54</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 183</t>
+          <t>Total filas: 194</t>
         </is>
       </c>
     </row>
@@ -1453,7 +1453,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1463,11 +1463,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1478,7 +1478,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1488,11 +1488,11 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1938,11 +1938,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2103,7 +2103,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2113,11 +2113,11 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>10:32:07</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3463,7 +3463,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D125" t="n">
@@ -3488,7 +3488,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D126" t="n">
@@ -3663,7 +3663,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D133" t="n">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -3728,7 +3728,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -3738,11 +3738,11 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3763,7 +3763,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D137" t="n">
@@ -3778,7 +3778,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3788,11 +3788,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3828,7 +3828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3838,11 +3838,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3863,11 +3863,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4553,12 +4553,12 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>14:44:54</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>14:47</t>
+          <t>14:46</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -4567,7 +4567,7 @@
         </is>
       </c>
       <c r="D169" t="n">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4578,12 +4578,12 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>14:48</t>
+          <t>14:47</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -4592,7 +4592,7 @@
         </is>
       </c>
       <c r="D170" t="n">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4608,16 +4608,16 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>14:51</t>
+          <t>14:48</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4628,7 +4628,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>14:44:54</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -4638,11 +4638,11 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4653,21 +4653,21 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>14:44:54</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>14:54</t>
+          <t>14:51</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4678,21 +4678,21 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>14:44:54</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>15:02</t>
+          <t>14:53</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4703,21 +4703,21 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>15:11</t>
+          <t>14:54</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>103</v>
+        <v>37</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4728,21 +4728,21 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>14:44:54</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>15:13</t>
+          <t>15:01</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4753,21 +4753,21 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>15:17</t>
+          <t>15:02</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4778,12 +4778,12 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>15:18</t>
+          <t>15:11</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -4792,7 +4792,7 @@
         </is>
       </c>
       <c r="D178" t="n">
-        <v>61</v>
+        <v>103</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4803,21 +4803,21 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>14:44:54</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>15:29</t>
+          <t>15:13</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4828,21 +4828,21 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>14:44:54</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>15:34</t>
+          <t>15:16</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D180" t="n">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -4853,21 +4853,21 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>14:44:54</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>15:36</t>
+          <t>15:17</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D181" t="n">
-        <v>79</v>
+        <v>33</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4878,21 +4878,21 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>15:41</t>
+          <t>15:18</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>107</v>
+        <v>61</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -4908,16 +4908,16 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>15:42</t>
+          <t>15:29</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D183" t="n">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -4928,21 +4928,21 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>14:44:54</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:33</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4958,16 +4958,16 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:34</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -4983,16 +4983,16 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>15:57</t>
+          <t>15:36</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5003,21 +5003,21 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>14:44:54</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>16:06</t>
+          <t>15:41</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5033,18 +5033,293 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
+          <t>15:42</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D188" t="n">
+        <v>85</v>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>14:44:54</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D189" t="n">
+        <v>69</v>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>14:44:54</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D190" t="n">
+        <v>69</v>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>14:44:54</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>15:54</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D191" t="n">
+        <v>70</v>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>14:17:13</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>15:57</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D192" t="n">
+        <v>100</v>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>14:44:54</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>16:05</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D193" t="n">
+        <v>81</v>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>14:17:13</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>16:06</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D194" t="n">
+        <v>109</v>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>14:44:54</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
           <t>16:14</t>
         </is>
       </c>
-      <c r="C188" t="inlineStr">
+      <c r="C195" t="inlineStr">
         <is>
           <t>17_ROMERO</t>
         </is>
       </c>
-      <c r="D188" t="n">
-        <v>117</v>
-      </c>
-      <c r="E188" t="inlineStr">
+      <c r="D195" t="n">
+        <v>90</v>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>14:44:54</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>16:16</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D196" t="n">
+        <v>92</v>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>14:44:54</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>16:21</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D197" t="n">
+        <v>97</v>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>14:44:54</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>16:34</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>83_ALUAR</t>
+        </is>
+      </c>
+      <c r="D198" t="n">
+        <v>110</v>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>14:44:54</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>16:40</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D199" t="n">
+        <v>116</v>
+      </c>
+      <c r="E199" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5061,7 +5336,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5079,14 +5354,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:17:13</t>
+          <t>Última actualización: 14:44:54</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 30</t>
+          <t>Total filas: 33</t>
         </is>
       </c>
     </row>
@@ -5770,12 +6045,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>14:44:54</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>14:47</t>
+          <t>14:46</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -5784,7 +6059,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -5795,12 +6070,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>14:48</t>
+          <t>14:47</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -5809,7 +6084,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -5825,16 +6100,16 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>14:54</t>
+          <t>14:48</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -5845,23 +6120,98 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
+          <t>14:44:54</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>9</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
           <t>14:17:13</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>14:54</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>37</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>14:44:54</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>15:33</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>49</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>14:17:13</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
         <is>
           <t>15:34</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D35" t="n">
+      <c r="D38" t="n">
         <v>77</v>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="E38" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5878,7 +6228,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5896,14 +6246,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:17:13</t>
+          <t>Última actualización: 14:44:54</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 30</t>
+          <t>Total filas: 33</t>
         </is>
       </c>
     </row>
@@ -6347,7 +6697,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -6372,7 +6722,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -6637,12 +6987,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>14:44:54</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>15:22</t>
+          <t>15:21</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -6651,7 +7001,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -6667,20 +7017,95 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
+          <t>15:22</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>65</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>14:44:54</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>16:01</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>77</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>14:17:13</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
           <t>16:02</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D35" t="n">
+      <c r="D37" t="n">
         <v>105</v>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>14:44:54</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>16:29</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>105</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1293
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E199"/>
+  <dimension ref="A1:E205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:44:54</t>
+          <t>Última actualización: 14:58:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 194</t>
+          <t>Total filas: 200</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1203,7 +1203,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1213,11 +1213,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1228,7 +1228,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1238,11 +1238,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,7 +1428,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1438,11 +1438,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2103,7 +2103,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2113,11 +2113,11 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D90" t="n">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D91" t="n">
@@ -3378,7 +3378,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -3388,11 +3388,11 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3403,7 +3403,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -3413,11 +3413,11 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -3728,7 +3728,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -3738,11 +3738,11 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3763,7 +3763,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D137" t="n">
@@ -3778,7 +3778,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3788,11 +3788,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3828,7 +3828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3838,11 +3838,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3863,11 +3863,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4053,7 +4053,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -4063,11 +4063,11 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4388,7 +4388,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D162" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4767,7 +4767,7 @@
         </is>
       </c>
       <c r="D177" t="n">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4803,7 +4803,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>14:44:54</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -4817,7 +4817,7 @@
         </is>
       </c>
       <c r="D179" t="n">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4828,7 +4828,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>14:44:54</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
@@ -4842,7 +4842,7 @@
         </is>
       </c>
       <c r="D180" t="n">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -4853,7 +4853,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>14:44:54</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -4867,7 +4867,7 @@
         </is>
       </c>
       <c r="D181" t="n">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4928,7 +4928,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>14:44:54</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4942,7 +4942,7 @@
         </is>
       </c>
       <c r="D184" t="n">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4992,7 +4992,7 @@
         </is>
       </c>
       <c r="D186" t="n">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>14:44:54</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5017,7 +5017,7 @@
         </is>
       </c>
       <c r="D187" t="n">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5053,7 +5053,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>14:44:54</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -5067,7 +5067,7 @@
         </is>
       </c>
       <c r="D189" t="n">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -5078,7 +5078,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>14:44:54</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
@@ -5092,7 +5092,7 @@
         </is>
       </c>
       <c r="D190" t="n">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -5128,12 +5128,12 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>15:57</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -5142,7 +5142,7 @@
         </is>
       </c>
       <c r="D192" t="n">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -5153,21 +5153,21 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>14:44:54</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>16:05</t>
+          <t>15:57</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,21 +5178,21 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>16:06</t>
+          <t>16:01</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>109</v>
+        <v>63</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5203,21 +5203,21 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>14:44:54</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>16:14</t>
+          <t>16:05</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5228,21 +5228,21 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>14:44:54</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>16:16</t>
+          <t>16:06</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D196" t="n">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -5253,21 +5253,21 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>14:44:54</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:14</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D197" t="n">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -5283,16 +5283,16 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:16</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>83_ALUAR</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D198" t="n">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5303,23 +5303,173 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
+          <t>14:58:38</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>16:17</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D199" t="n">
+        <v>79</v>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>14:58:38</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>16:21</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D200" t="n">
+        <v>83</v>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>14:58:38</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>16:34</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>83_ALUAR</t>
+        </is>
+      </c>
+      <c r="D201" t="n">
+        <v>96</v>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
           <t>14:44:54</t>
         </is>
       </c>
-      <c r="B199" t="inlineStr">
+      <c r="B202" t="inlineStr">
         <is>
           <t>16:40</t>
         </is>
       </c>
-      <c r="C199" t="inlineStr">
+      <c r="C202" t="inlineStr">
         <is>
           <t>225_GOMEZ</t>
         </is>
       </c>
-      <c r="D199" t="n">
+      <c r="D202" t="n">
         <v>116</v>
       </c>
-      <c r="E199" t="inlineStr">
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>14:58:38</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>16:41</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D203" t="n">
+        <v>103</v>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>14:58:38</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>16:46</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D204" t="n">
+        <v>108</v>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>14:58:38</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>16:53</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D205" t="n">
+        <v>115</v>
+      </c>
+      <c r="E205" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5354,7 +5504,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:44:54</t>
+          <t>Última actualización: 14:58:38</t>
         </is>
       </c>
     </row>
@@ -6170,7 +6320,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>14:44:54</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -6184,7 +6334,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -6228,7 +6378,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6246,14 +6396,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:44:54</t>
+          <t>Última actualización: 14:58:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 33</t>
+          <t>Total filas: 34</t>
         </is>
       </c>
     </row>
@@ -6697,7 +6847,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -6722,7 +6872,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -6987,7 +7137,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>14:44:54</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -7001,7 +7151,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -7037,7 +7187,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>14:44:54</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -7051,7 +7201,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -7104,6 +7254,31 @@
         <v>105</v>
       </c>
       <c r="E38" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>14:58:38</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>92</v>
+      </c>
+      <c r="E39" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1294
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E205"/>
+  <dimension ref="A1:E216"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:58:38</t>
+          <t>Última actualización: 15:34:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 200</t>
+          <t>Total filas: 211</t>
         </is>
       </c>
     </row>
@@ -903,7 +903,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -913,11 +913,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -938,11 +938,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1203,7 +1203,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1213,11 +1213,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1228,7 +1228,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1238,11 +1238,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,7 +1428,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1438,11 +1438,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>10:32:07</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3763,7 +3763,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D137" t="n">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -3828,7 +3828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3838,11 +3838,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3863,11 +3863,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4053,7 +4053,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -4063,11 +4063,11 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4953,7 +4953,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4967,7 +4967,7 @@
         </is>
       </c>
       <c r="D185" t="n">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -5028,21 +5028,21 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>15:42</t>
+          <t>15:41</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5053,21 +5053,21 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:42</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D189" t="n">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -5078,7 +5078,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
@@ -5088,11 +5088,11 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D190" t="n">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -5103,21 +5103,21 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>14:44:54</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>15:54</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -5128,21 +5128,21 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -5153,12 +5153,12 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>14:44:54</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>15:57</t>
+          <t>15:54</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -5167,7 +5167,7 @@
         </is>
       </c>
       <c r="D193" t="n">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5183,16 +5183,16 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>16:01</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5203,21 +5203,21 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>16:05</t>
+          <t>15:57</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5228,21 +5228,21 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>16:06</t>
+          <t>16:01</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D196" t="n">
-        <v>109</v>
+        <v>63</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -5253,21 +5253,21 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>16:14</t>
+          <t>16:05</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D197" t="n">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -5278,21 +5278,21 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>14:44:54</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>16:16</t>
+          <t>16:05</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D198" t="n">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5303,21 +5303,21 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>16:17</t>
+          <t>16:06</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>79</v>
+        <v>32</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5328,21 +5328,21 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:14</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -5353,21 +5353,21 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>14:44:54</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:16</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>83_ALUAR</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5378,21 +5378,21 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>14:44:54</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>16:40</t>
+          <t>16:17</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D202" t="n">
-        <v>116</v>
+        <v>43</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -5403,21 +5403,21 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>16:41</t>
+          <t>16:18</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D203" t="n">
-        <v>103</v>
+        <v>44</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -5433,16 +5433,16 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>16:46</t>
+          <t>16:21</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D204" t="n">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -5453,23 +5453,298 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
+          <t>15:34:15</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D205" t="n">
+        <v>56</v>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>15:34:15</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>16:34</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>83_ALUAR</t>
+        </is>
+      </c>
+      <c r="D206" t="n">
+        <v>60</v>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>14:44:54</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>16:40</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D207" t="n">
+        <v>116</v>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>15:34:15</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>16:41</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D208" t="n">
+        <v>67</v>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>15:34:15</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>16:46</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D209" t="n">
+        <v>72</v>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>15:34:15</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>16:52</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D210" t="n">
+        <v>78</v>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
           <t>14:58:38</t>
         </is>
       </c>
-      <c r="B205" t="inlineStr">
+      <c r="B211" t="inlineStr">
         <is>
           <t>16:53</t>
         </is>
       </c>
-      <c r="C205" t="inlineStr">
+      <c r="C211" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D205" t="n">
+      <c r="D211" t="n">
         <v>115</v>
       </c>
-      <c r="E205" t="inlineStr">
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>15:34:15</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>16:54</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D212" t="n">
+        <v>80</v>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>15:34:15</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>16:58</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D213" t="n">
+        <v>84</v>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>15:34:15</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>17:07</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D214" t="n">
+        <v>93</v>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>15:34:15</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>17:10</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D215" t="n">
+        <v>96</v>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>15:34:15</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>17:21</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D216" t="n">
+        <v>107</v>
+      </c>
+      <c r="E216" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5481,898 +5756,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E38"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>LÍNEA 141 - LP1912-215 - 01/02/2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Última actualización: 14:58:38</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Total filas: 33</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Hora_Scrap</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Hora_Llegada</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Linea</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Minutos</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Parada</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>06:15:23</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>06:16</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>06:46:40</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>06:56</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>10</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>06:15:23</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>06:57</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>42</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>06:58:58</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>06:58</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>06:58:58</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>07:15</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>17</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>06:15:23</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>07:16</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>61</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>07:26:49</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>07:43</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>17</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>08:14:55</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>08:43</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>29</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>08:35:17</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>08:44</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>9</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>08:49:06</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>08:50</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>08:14:55</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>08:53</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>39</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>08:49:06</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>08:54</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>5</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>08:14:55</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>08:57</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>43</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>08:57:42</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>08:58</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>1</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>09:42:42</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>09:58</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>16</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>08:49:06</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>09:59</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>70</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>09:42:42</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>11:30</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>108</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>11:01:19</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>11:31</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>30</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>11:01:19</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>11:41</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>40</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>11:38:09</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>11:42</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>4</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>12:18:38</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>12:21</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>3</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>11:56:32</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>12:22</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>26</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>12:18:38</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>13:03</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>45</v>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>12:58:23</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>13:04</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>6</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>13:28:27</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>13:33</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
-        <v>5</v>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>14:17:13</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>14:34</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v>17</v>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>14:44:54</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>14:46</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D32" t="n">
-        <v>2</v>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>13:54:35</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>14:47</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
-        <v>53</v>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>14:17:13</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>14:48</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
-        <v>31</v>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>14:44:54</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>14:53</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>215_EL PELIGRO</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
-        <v>9</v>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>14:17:13</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>14:54</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>215_EL PELIGRO</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
-        <v>37</v>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>14:58:38</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>15:33</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
-        <v>35</v>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>14:17:13</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>15:34</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D38" t="n">
-        <v>77</v>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6389,14 +5772,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - 6203-6173 - 01/02/2026</t>
+          <t>LÍNEA 141 - LP1912-215 - 01/02/2026</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:58:38</t>
+          <t>Última actualización: 15:34:15</t>
         </is>
       </c>
     </row>
@@ -6437,6 +5820,923 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>06:15:23</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>06:16</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>06:46:40</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>06:56</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>10</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>06:15:23</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>06:57</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>42</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>06:58:58</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>06:58</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>06:58:58</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>07:15</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>17</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>06:15:23</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>07:16</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>61</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>07:26:49</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>07:43</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>17</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>08:14:55</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>08:43</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>29</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>08:35:17</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>9</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>08:49:06</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>08:50</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>08:14:55</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>08:53</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>39</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>08:49:06</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>08:54</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>5</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>08:14:55</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>08:57</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>43</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>08:57:42</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>08:58</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>09:42:42</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>09:58</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>16</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>08:49:06</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>09:59</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>70</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>09:42:42</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>108</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>11:01:19</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>11:31</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>30</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>11:01:19</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>11:41</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>40</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>11:38:09</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>11:42</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>4</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>12:18:38</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>3</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>11:56:32</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>12:22</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>26</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>12:18:38</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13:03</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>45</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>12:58:23</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>6</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>13:28:27</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>13:33</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>5</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>14:17:13</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>17</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>14:44:54</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>14:46</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>2</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>13:54:35</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>14:47</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>53</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>14:17:13</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>14:48</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>31</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>14:44:54</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>9</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>14:17:13</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>14:54</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>37</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>14:58:38</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>15:33</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>35</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>15:34:15</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>15:34:15</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>17:10</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>96</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LÍNEA 141 - 6203-6173 - 01/02/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Última actualización: 15:34:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Total filas: 35</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>07:26:49</t>
         </is>
       </c>
@@ -6847,7 +7147,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -6872,7 +7172,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -7212,7 +7512,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -7226,7 +7526,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>105</v>
+        <v>28</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -7262,7 +7562,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -7276,11 +7576,36 @@
         </is>
       </c>
       <c r="D39" t="n">
+        <v>56</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>15:34:15</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>17:06</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
         <v>92</v>
       </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>L6173</t>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1295
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E216"/>
+  <dimension ref="A1:E225"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:34:15</t>
+          <t>Última actualización: 16:02:30</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 211</t>
+          <t>Total filas: 220</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1203,7 +1203,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1213,11 +1213,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1228,7 +1228,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1238,11 +1238,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,7 +1428,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1438,11 +1438,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -3263,7 +3263,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D117" t="n">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3763,7 +3763,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D137" t="n">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5138,7 +5138,7 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D192" t="n">
@@ -5253,12 +5253,12 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>16:05</t>
+          <t>16:02</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
@@ -5267,7 +5267,7 @@
         </is>
       </c>
       <c r="D197" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -5278,12 +5278,12 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>16:05</t>
+          <t>16:04</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
@@ -5292,7 +5292,7 @@
         </is>
       </c>
       <c r="D198" t="n">
-        <v>67</v>
+        <v>2</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5303,21 +5303,21 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>16:06</t>
+          <t>16:05</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5328,21 +5328,21 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>16:14</t>
+          <t>16:05</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -5353,21 +5353,21 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>14:44:54</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>16:16</t>
+          <t>16:06</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5378,21 +5378,21 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>16:17</t>
+          <t>16:14</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D202" t="n">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -5403,21 +5403,21 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>14:44:54</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>16:18</t>
+          <t>16:16</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D203" t="n">
-        <v>44</v>
+        <v>92</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -5428,21 +5428,21 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:17</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D204" t="n">
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -5458,16 +5458,16 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:18</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D205" t="n">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -5478,21 +5478,21 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:21</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>83_ALUAR</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D206" t="n">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -5503,21 +5503,21 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>14:44:54</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>16:40</t>
+          <t>16:29</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>116</v>
+        <v>27</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5533,16 +5533,16 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>16:41</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5553,21 +5553,21 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>16:46</t>
+          <t>16:34</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>83_ALUAR</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5578,21 +5578,21 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>14:44:54</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>16:52</t>
+          <t>16:40</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>78</v>
+        <v>116</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5603,21 +5603,21 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:41</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>115</v>
+        <v>39</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -5633,16 +5633,16 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>16:54</t>
+          <t>16:46</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5658,16 +5658,16 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>16:58</t>
+          <t>16:52</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,21 +5678,21 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>93</v>
+        <v>51</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5708,16 +5708,16 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>17:10</t>
+          <t>16:54</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D215" t="n">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -5728,23 +5728,248 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
+          <t>16:58</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D216" t="n">
+        <v>56</v>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>16:02:30</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>17:07</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D217" t="n">
+        <v>65</v>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>16:02:30</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>17:10</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D218" t="n">
+        <v>68</v>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>16:02:30</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>17:17</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D219" t="n">
+        <v>75</v>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>16:02:30</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
           <t>17:21</t>
         </is>
       </c>
-      <c r="C216" t="inlineStr">
+      <c r="C220" t="inlineStr">
         <is>
           <t>15X38_ABASTO</t>
         </is>
       </c>
-      <c r="D216" t="n">
+      <c r="D220" t="n">
+        <v>79</v>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>16:02:30</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>17:34</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D221" t="n">
+        <v>92</v>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>16:02:30</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>17:36</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D222" t="n">
+        <v>94</v>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>16:02:30</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D223" t="n">
+        <v>96</v>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>16:02:30</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>17:44</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D224" t="n">
+        <v>102</v>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>16:02:30</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>17:49</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D225" t="n">
         <v>107</v>
       </c>
-      <c r="E216" t="inlineStr">
+      <c r="E225" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5761,7 +5986,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5779,14 +6004,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:34:15</t>
+          <t>Última actualización: 16:02:30</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 34</t>
+          <t>Total filas: 36</t>
         </is>
       </c>
     </row>
@@ -6645,7 +6870,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -6659,9 +6884,59 @@
         </is>
       </c>
       <c r="D39" t="n">
+        <v>68</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>16:02:30</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
         <v>96</v>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>16:02:30</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>17:44</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>102</v>
+      </c>
+      <c r="E41" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6696,7 +6971,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:34:15</t>
+          <t>Última actualización: 16:02:30</t>
         </is>
       </c>
     </row>
@@ -7512,7 +7787,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -7526,7 +7801,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -7562,7 +7837,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -7576,7 +7851,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -7587,7 +7862,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -7601,7 +7876,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1296
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E225"/>
+  <dimension ref="A1:E239"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:02:30</t>
+          <t>Última actualización: 16:34:05</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 220</t>
+          <t>Total filas: 234</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1453,7 +1453,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1463,11 +1463,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1478,7 +1478,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1488,11 +1488,11 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -3378,7 +3378,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -3388,11 +3388,11 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3403,7 +3403,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -3413,11 +3413,11 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D133" t="n">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D191" t="n">
@@ -5138,7 +5138,7 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D192" t="n">
@@ -5303,7 +5303,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -5313,11 +5313,11 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5328,7 +5328,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -5338,11 +5338,11 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -5553,7 +5553,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -5567,7 +5567,7 @@
         </is>
       </c>
       <c r="D209" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5578,21 +5578,21 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>14:44:54</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>16:40</t>
+          <t>16:35</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>116</v>
+        <v>1</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5603,12 +5603,12 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>14:44:54</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>16:41</t>
+          <t>16:40</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
@@ -5617,7 +5617,7 @@
         </is>
       </c>
       <c r="D211" t="n">
-        <v>39</v>
+        <v>116</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -5628,21 +5628,21 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>16:46</t>
+          <t>16:41</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5658,16 +5658,16 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>16:52</t>
+          <t>16:46</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,21 +5678,21 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:52</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5703,12 +5703,12 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>16:54</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
@@ -5717,7 +5717,7 @@
         </is>
       </c>
       <c r="D215" t="n">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -5728,21 +5728,21 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>16:58</t>
+          <t>16:54</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -5753,21 +5753,21 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>16:55</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -5778,21 +5778,21 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>17:10</t>
+          <t>16:58</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -5803,12 +5803,12 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>17:17</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -5817,7 +5817,7 @@
         </is>
       </c>
       <c r="D219" t="n">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -5828,21 +5828,21 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D220" t="n">
-        <v>79</v>
+        <v>33</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -5853,21 +5853,21 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D221" t="n">
-        <v>92</v>
+        <v>36</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -5883,16 +5883,16 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:17</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D222" t="n">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -5903,21 +5903,21 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,21 +5928,21 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>102</v>
+        <v>60</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5953,23 +5953,373 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
+          <t>16:34:05</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>17:34</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D225" t="n">
+        <v>60</v>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
           <t>16:02:30</t>
         </is>
       </c>
-      <c r="B225" t="inlineStr">
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>17:36</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D226" t="n">
+        <v>94</v>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>16:02:30</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D227" t="n">
+        <v>96</v>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>16:34:05</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>17:39</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D228" t="n">
+        <v>65</v>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>16:02:30</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>17:44</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D229" t="n">
+        <v>102</v>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>16:34:05</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>17:46</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D230" t="n">
+        <v>72</v>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>16:34:05</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
         <is>
           <t>17:49</t>
         </is>
       </c>
-      <c r="C225" t="inlineStr">
+      <c r="C231" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D225" t="n">
-        <v>107</v>
-      </c>
-      <c r="E225" t="inlineStr">
+      <c r="D231" t="n">
+        <v>75</v>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>16:34:05</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>17:53</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D232" t="n">
+        <v>79</v>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>16:34:05</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>17:58</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D233" t="n">
+        <v>84</v>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>16:34:05</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>18:06</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D234" t="n">
+        <v>92</v>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>16:34:05</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>18:10</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D235" t="n">
+        <v>96</v>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>16:34:05</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>18:10</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D236" t="n">
+        <v>96</v>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>16:34:05</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>18:17</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D237" t="n">
+        <v>103</v>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>16:34:05</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D238" t="n">
+        <v>108</v>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>16:34:05</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>18:30</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D239" t="n">
+        <v>116</v>
+      </c>
+      <c r="E239" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5986,7 +6336,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6004,14 +6354,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:02:30</t>
+          <t>Última actualización: 16:34:05</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 36</t>
+          <t>Total filas: 39</t>
         </is>
       </c>
     </row>
@@ -6870,7 +7220,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -6884,7 +7234,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -6920,23 +7270,98 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>16:34:05</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>17:39</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>65</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
           <t>16:02:30</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B42" t="inlineStr">
         <is>
           <t>17:44</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>215_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D41" t="n">
+      <c r="D42" t="n">
         <v>102</v>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>16:34:05</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>17:46</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>72</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>16:34:05</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>108</v>
+      </c>
+      <c r="E44" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6971,7 +7396,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:02:30</t>
+          <t>Última actualización: 16:34:05</t>
         </is>
       </c>
     </row>
@@ -7422,7 +7847,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -7447,7 +7872,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -7862,7 +8287,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -7876,7 +8301,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1297
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E239"/>
+  <dimension ref="A1:E248"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:34:05</t>
+          <t>Última actualización: 16:49:34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 234</t>
+          <t>Total filas: 243</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1938,11 +1938,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>10:32:07</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3378,7 +3378,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -3388,11 +3388,11 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3403,7 +3403,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -3413,11 +3413,11 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3463,7 +3463,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D125" t="n">
@@ -3488,7 +3488,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D126" t="n">
@@ -3828,7 +3828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3838,11 +3838,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3863,11 +3863,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5678,12 +5678,12 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>16:49:34</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>16:52</t>
+          <t>16:49</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
@@ -5692,7 +5692,7 @@
         </is>
       </c>
       <c r="D214" t="n">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5703,12 +5703,12 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>16:49:34</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:51</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
@@ -5717,7 +5717,7 @@
         </is>
       </c>
       <c r="D215" t="n">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -5728,21 +5728,21 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>16:54</t>
+          <t>16:52</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -5753,21 +5753,21 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>16:55</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -5783,16 +5783,16 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>16:58</t>
+          <t>16:54</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -5808,16 +5808,16 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>16:55</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D219" t="n">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -5828,21 +5828,21 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:49:34</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>16:58</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D220" t="n">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -5853,21 +5853,21 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:49:34</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>17:10</t>
+          <t>17:06</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D221" t="n">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -5878,21 +5878,21 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>16:49:34</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>17:17</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D222" t="n">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -5908,16 +5908,16 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,21 +5928,21 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:49:34</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5953,21 +5953,21 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:17</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5978,21 +5978,21 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>16:49:34</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>94</v>
+        <v>32</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6003,21 +6003,21 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D227" t="n">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -6028,21 +6028,21 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:49:34</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>17:39</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6053,21 +6053,21 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>16:49:34</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>102</v>
+        <v>47</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,21 +6078,21 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:49:34</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>17:46</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6108,16 +6108,16 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>17:49</t>
+          <t>17:39</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6128,21 +6128,21 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>17:53</t>
+          <t>17:44</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6153,21 +6153,21 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:49:34</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>17:58</t>
+          <t>17:46</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D233" t="n">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -6183,16 +6183,16 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>18:06</t>
+          <t>17:49</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D234" t="n">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -6203,21 +6203,21 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:49:34</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D235" t="n">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -6228,21 +6228,21 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:49:34</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D236" t="n">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -6258,16 +6258,16 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>18:17</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D237" t="n">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -6278,21 +6278,21 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:49:34</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>18:22</t>
+          <t>17:58</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>108</v>
+        <v>69</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -6303,23 +6303,248 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
+          <t>16:49:34</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>18:05</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D239" t="n">
+        <v>76</v>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
           <t>16:34:05</t>
         </is>
       </c>
-      <c r="B239" t="inlineStr">
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>18:06</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D240" t="n">
+        <v>92</v>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>16:49:34</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>18:10</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D241" t="n">
+        <v>81</v>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>16:49:34</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>18:10</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D242" t="n">
+        <v>81</v>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>16:49:34</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>18:17</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D243" t="n">
+        <v>88</v>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>16:49:34</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D244" t="n">
+        <v>93</v>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>16:49:34</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>18:25</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D245" t="n">
+        <v>96</v>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>16:49:34</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>18:29</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D246" t="n">
+        <v>100</v>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>16:34:05</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
         <is>
           <t>18:30</t>
         </is>
       </c>
-      <c r="C239" t="inlineStr">
+      <c r="C247" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D239" t="n">
+      <c r="D247" t="n">
         <v>116</v>
       </c>
-      <c r="E239" t="inlineStr">
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>16:49:34</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>18:36</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D248" t="n">
+        <v>107</v>
+      </c>
+      <c r="E248" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6354,7 +6579,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:34:05</t>
+          <t>Última actualización: 16:49:34</t>
         </is>
       </c>
     </row>
@@ -7220,7 +7445,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:49:34</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -7234,7 +7459,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -7245,7 +7470,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>16:49:34</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -7259,7 +7484,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -7320,7 +7545,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:49:34</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -7334,7 +7559,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -7345,7 +7570,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:49:34</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -7359,7 +7584,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -7378,7 +7603,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7396,14 +7621,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:34:05</t>
+          <t>Última actualización: 16:49:34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 35</t>
+          <t>Total filas: 37</t>
         </is>
       </c>
     </row>
@@ -7762,7 +7987,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -7772,11 +7997,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>101</v>
+        <v>48</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -7787,7 +8012,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>09:42:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -7797,11 +8022,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -7847,7 +8072,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -7872,7 +8097,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -8287,23 +8512,73 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
+          <t>16:49:34</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>16</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
           <t>16:34:05</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B41" t="inlineStr">
         <is>
           <t>17:06</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C41" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D40" t="n">
+      <c r="D41" t="n">
         <v>32</v>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>16:49:34</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>18:35</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>106</v>
+      </c>
+      <c r="E42" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1298
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E248"/>
+  <dimension ref="A1:E254"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:49:34</t>
+          <t>Última actualización: 16:57:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 243</t>
+          <t>Total filas: 249</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -903,7 +903,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -913,11 +913,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -938,11 +938,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1203,7 +1203,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1213,11 +1213,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1228,7 +1228,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1238,11 +1238,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,7 +1428,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1438,11 +1438,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1453,7 +1453,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1463,11 +1463,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1478,7 +1478,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1488,11 +1488,11 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1938,11 +1938,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D90" t="n">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D91" t="n">
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>10:32:07</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3378,7 +3378,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -3388,11 +3388,11 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3403,7 +3403,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -3413,11 +3413,11 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3463,7 +3463,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D125" t="n">
@@ -3488,7 +3488,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D126" t="n">
@@ -3728,7 +3728,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -3738,11 +3738,11 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3763,7 +3763,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D137" t="n">
@@ -3778,7 +3778,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3788,11 +3788,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4388,7 +4388,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D162" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4638,7 +4638,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D172" t="n">
@@ -4663,7 +4663,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D173" t="n">
@@ -5303,7 +5303,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -5313,11 +5313,11 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5328,7 +5328,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -5338,11 +5338,11 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -5828,21 +5828,21 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>16:58</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D220" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -5853,21 +5853,21 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>17:06</t>
+          <t>16:58</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D221" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -5878,21 +5878,21 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>17:06</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D222" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -5928,21 +5928,21 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>17:10</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5953,21 +5953,21 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>17:17</t>
+          <t>17:09</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>75</v>
+        <v>12</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5983,16 +5983,16 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6003,21 +6003,21 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:17</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D227" t="n">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -6028,21 +6028,21 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6053,12 +6053,12 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
@@ -6067,7 +6067,7 @@
         </is>
       </c>
       <c r="D229" t="n">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,21 +6078,21 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6103,21 +6103,21 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>17:39</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6128,21 +6128,21 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6153,21 +6153,21 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>17:46</t>
+          <t>17:39</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D233" t="n">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -6178,21 +6178,21 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>17:49</t>
+          <t>17:44</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D234" t="n">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -6203,21 +6203,21 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D235" t="n">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -6233,16 +6233,16 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>17:53</t>
+          <t>17:46</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D236" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -6253,12 +6253,12 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>17:53</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
@@ -6267,7 +6267,7 @@
         </is>
       </c>
       <c r="D237" t="n">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -6278,21 +6278,21 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>17:58</t>
+          <t>17:49</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -6308,16 +6308,16 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D239" t="n">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -6328,21 +6328,21 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>18:06</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6353,21 +6353,21 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,21 +6378,21 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>17:58</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6403,21 +6403,21 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>18:17</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6428,21 +6428,21 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>18:22</t>
+          <t>18:06</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6453,21 +6453,21 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>18:25</t>
+          <t>18:10</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -6478,21 +6478,21 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>18:29</t>
+          <t>18:10</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D246" t="n">
-        <v>100</v>
+        <v>73</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -6503,21 +6503,21 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:49:34</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>18:30</t>
+          <t>18:17</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D247" t="n">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -6528,23 +6528,173 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
+          <t>16:57:38</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D248" t="n">
+        <v>84</v>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
           <t>16:49:34</t>
         </is>
       </c>
-      <c r="B248" t="inlineStr">
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D249" t="n">
+        <v>93</v>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>16:57:38</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>18:23</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D250" t="n">
+        <v>86</v>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>16:57:38</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>18:25</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D251" t="n">
+        <v>88</v>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>16:57:38</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>18:29</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D252" t="n">
+        <v>92</v>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>16:34:05</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>18:30</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D253" t="n">
+        <v>116</v>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>16:57:38</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
         <is>
           <t>18:36</t>
         </is>
       </c>
-      <c r="C248" t="inlineStr">
+      <c r="C254" t="inlineStr">
         <is>
           <t>15X38_ABASTO</t>
         </is>
       </c>
-      <c r="D248" t="n">
-        <v>107</v>
-      </c>
-      <c r="E248" t="inlineStr">
+      <c r="D254" t="n">
+        <v>99</v>
+      </c>
+      <c r="E254" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6561,7 +6711,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6579,14 +6729,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:49:34</t>
+          <t>Última actualización: 16:57:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 39</t>
+          <t>Total filas: 42</t>
         </is>
       </c>
     </row>
@@ -7445,12 +7595,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>17:10</t>
+          <t>17:09</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -7459,7 +7609,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -7475,16 +7625,16 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -7495,12 +7645,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>17:39</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -7509,7 +7659,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -7520,21 +7670,21 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>17:39</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>102</v>
+        <v>65</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -7545,12 +7695,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>17:46</t>
+          <t>17:44</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -7559,7 +7709,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -7570,23 +7720,98 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
+          <t>16:57:38</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>48</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
           <t>16:49:34</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>17:46</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>57</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>16:57:38</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>84</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>16:49:34</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
         <is>
           <t>18:22</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="C47" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D44" t="n">
+      <c r="D47" t="n">
         <v>93</v>
       </c>
-      <c r="E44" t="inlineStr">
+      <c r="E47" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7621,7 +7846,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:49:34</t>
+          <t>Última actualización: 16:57:38</t>
         </is>
       </c>
     </row>
@@ -7987,7 +8212,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>09:42:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -7997,11 +8222,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -8012,7 +8237,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -8022,11 +8247,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>101</v>
+        <v>48</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -8512,7 +8737,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -8526,7 +8751,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -8562,7 +8787,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -8576,7 +8801,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1299
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E254"/>
+  <dimension ref="A1:E264"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:57:38</t>
+          <t>Última actualización: 17:22:11</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 249</t>
+          <t>Total filas: 259</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1203,7 +1203,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1213,11 +1213,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1228,7 +1228,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1238,11 +1238,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,7 +1428,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1438,11 +1438,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D90" t="n">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D91" t="n">
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>10:32:07</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3263,7 +3263,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D117" t="n">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3463,7 +3463,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D125" t="n">
@@ -3488,7 +3488,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D126" t="n">
@@ -3663,7 +3663,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -3728,7 +3728,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -3738,11 +3738,11 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3763,7 +3763,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D137" t="n">
@@ -3778,7 +3778,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3788,11 +3788,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3828,7 +3828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3838,11 +3838,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3863,11 +3863,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D191" t="n">
@@ -5303,7 +5303,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -5313,11 +5313,11 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5328,7 +5328,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -5338,11 +5338,11 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -6053,21 +6053,21 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:22</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>16:57:38</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6092,7 +6092,7 @@
         </is>
       </c>
       <c r="D230" t="n">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6103,12 +6103,12 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>16:57:38</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
@@ -6117,7 +6117,7 @@
         </is>
       </c>
       <c r="D231" t="n">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6133,16 +6133,16 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6153,21 +6153,21 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>17:39</t>
+          <t>17:37</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D233" t="n">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -6178,21 +6178,21 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D234" t="n">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -6203,21 +6203,21 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>16:57:38</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:39</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D235" t="n">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -6228,12 +6228,12 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>17:46</t>
+          <t>17:44</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
@@ -6242,7 +6242,7 @@
         </is>
       </c>
       <c r="D236" t="n">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -6258,16 +6258,16 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D237" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -6278,21 +6278,21 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>17:49</t>
+          <t>17:46</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -6303,12 +6303,12 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
@@ -6317,7 +6317,7 @@
         </is>
       </c>
       <c r="D239" t="n">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -6328,12 +6328,12 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>16:57:38</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>17:53</t>
+          <t>17:49</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
@@ -6342,7 +6342,7 @@
         </is>
       </c>
       <c r="D240" t="n">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6353,12 +6353,12 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>17:53</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
@@ -6367,7 +6367,7 @@
         </is>
       </c>
       <c r="D241" t="n">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,21 +6378,21 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>16:57:38</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>17:58</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6403,21 +6403,21 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>16:57:38</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6428,21 +6428,21 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>18:06</t>
+          <t>17:58</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>92</v>
+        <v>36</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6458,16 +6458,16 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -6478,21 +6478,21 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>16:57:38</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>18:06</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D246" t="n">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -6503,21 +6503,21 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>18:17</t>
+          <t>18:10</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D247" t="n">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -6528,21 +6528,21 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>16:57:38</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:10</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D248" t="n">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -6558,16 +6558,16 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>18:22</t>
+          <t>18:17</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D249" t="n">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -6583,16 +6583,16 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>18:23</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -6603,21 +6603,21 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>16:57:38</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>18:25</t>
+          <t>18:22</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -6633,16 +6633,16 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>18:29</t>
+          <t>18:23</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D252" t="n">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -6653,21 +6653,21 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>18:30</t>
+          <t>18:25</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D253" t="n">
-        <v>116</v>
+        <v>63</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -6683,18 +6683,268 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
+          <t>18:29</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D254" t="n">
+        <v>92</v>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>17:22:11</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>18:30</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D255" t="n">
+        <v>68</v>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>17:22:11</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
           <t>18:36</t>
         </is>
       </c>
-      <c r="C254" t="inlineStr">
+      <c r="C256" t="inlineStr">
         <is>
           <t>15X38_ABASTO</t>
         </is>
       </c>
-      <c r="D254" t="n">
-        <v>99</v>
-      </c>
-      <c r="E254" t="inlineStr">
+      <c r="D256" t="n">
+        <v>74</v>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>17:22:11</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>18:40</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D257" t="n">
+        <v>78</v>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>17:22:11</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>18:41</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D258" t="n">
+        <v>79</v>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>17:22:11</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>18:45</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D259" t="n">
+        <v>83</v>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>17:22:11</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>18:57</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D260" t="n">
+        <v>95</v>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>17:22:11</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D261" t="n">
+        <v>98</v>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>17:22:11</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D262" t="n">
+        <v>102</v>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>17:22:11</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D263" t="n">
+        <v>115</v>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>17:22:11</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D264" t="n">
+        <v>115</v>
+      </c>
+      <c r="E264" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6711,7 +6961,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6729,14 +6979,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:57:38</t>
+          <t>Última actualización: 17:22:11</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 42</t>
+          <t>Total filas: 43</t>
         </is>
       </c>
     </row>
@@ -7670,7 +7920,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -7684,7 +7934,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -7745,7 +7995,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -7759,7 +8009,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -7795,7 +8045,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -7809,9 +8059,34 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="E47" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>17:22:11</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>102</v>
+      </c>
+      <c r="E48" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7828,7 +8103,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7846,14 +8121,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:57:38</t>
+          <t>Última actualización: 17:22:11</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 37</t>
+          <t>Total filas: 38</t>
         </is>
       </c>
     </row>
@@ -8297,7 +8572,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -8322,7 +8597,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -8804,6 +9079,31 @@
         <v>98</v>
       </c>
       <c r="E42" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>17:22:11</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>18:36</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>74</v>
+      </c>
+      <c r="E43" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1300
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E264"/>
+  <dimension ref="A1:E273"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:22:11</t>
+          <t>Última actualización: 17:47:31</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 259</t>
+          <t>Total filas: 268</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -903,7 +903,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -913,11 +913,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -938,11 +938,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,7 +1428,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1438,11 +1438,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D90" t="n">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D91" t="n">
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>10:32:07</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3828,7 +3828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3838,11 +3838,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3863,11 +3863,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4053,7 +4053,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -4063,11 +4063,11 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4388,7 +4388,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D162" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4638,7 +4638,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D172" t="n">
@@ -4663,7 +4663,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D173" t="n">
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>16:57:38</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -6303,21 +6303,21 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>16:57:38</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D239" t="n">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -6328,21 +6328,21 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>17:49</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6353,21 +6353,21 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>17:49</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,12 +6378,12 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>17:53</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
@@ -6392,7 +6392,7 @@
         </is>
       </c>
       <c r="D242" t="n">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6403,12 +6403,12 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>17:53</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
@@ -6417,7 +6417,7 @@
         </is>
       </c>
       <c r="D243" t="n">
-        <v>79</v>
+        <v>4</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6433,16 +6433,16 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>17:58</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6453,21 +6453,21 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>16:57:38</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -6478,21 +6478,21 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>18:06</t>
+          <t>17:58</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D246" t="n">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -6503,21 +6503,21 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D247" t="n">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -6533,16 +6533,16 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>18:06</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D248" t="n">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -6553,21 +6553,21 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>18:17</t>
+          <t>18:10</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D249" t="n">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -6578,21 +6578,21 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>16:57:38</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:10</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -6603,21 +6603,21 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>16:49:34</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>18:22</t>
+          <t>18:17</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -6633,16 +6633,16 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>18:23</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D252" t="n">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -6653,21 +6653,21 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>18:25</t>
+          <t>18:22</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D253" t="n">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -6683,16 +6683,16 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>18:29</t>
+          <t>18:23</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D254" t="n">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -6703,21 +6703,21 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>18:30</t>
+          <t>18:25</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D255" t="n">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -6728,21 +6728,21 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>18:36</t>
+          <t>18:29</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D256" t="n">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -6758,16 +6758,16 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>18:30</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6778,21 +6778,21 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>18:41</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -6803,21 +6803,21 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>18:45</t>
+          <t>18:36</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D259" t="n">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -6833,16 +6833,16 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>18:57</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D260" t="n">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -6853,21 +6853,21 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:41</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6878,21 +6878,21 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:45</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>102</v>
+        <v>58</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -6903,21 +6903,21 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>115</v>
+        <v>65</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -6928,23 +6928,248 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
+          <t>17:47:31</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>18:57</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D264" t="n">
+        <v>70</v>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>17:47:31</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>18:59</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D265" t="n">
+        <v>72</v>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
           <t>17:22:11</t>
         </is>
       </c>
-      <c r="B264" t="inlineStr">
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D266" t="n">
+        <v>98</v>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>17:47:31</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D267" t="n">
+        <v>77</v>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>17:47:31</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
         <is>
           <t>19:17</t>
         </is>
       </c>
-      <c r="C264" t="inlineStr">
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D268" t="n">
+        <v>90</v>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>17:22:11</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="D264" t="n">
+      <c r="D269" t="n">
         <v>115</v>
       </c>
-      <c r="E264" t="inlineStr">
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>17:47:31</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>19:18</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D270" t="n">
+        <v>91</v>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>17:47:31</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>19:28</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D271" t="n">
+        <v>101</v>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>17:47:31</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>19:35</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D272" t="n">
+        <v>108</v>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>17:47:31</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D273" t="n">
+        <v>113</v>
+      </c>
+      <c r="E273" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6961,7 +7186,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6979,14 +7204,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:22:11</t>
+          <t>Última actualización: 17:47:31</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 43</t>
+          <t>Total filas: 45</t>
         </is>
       </c>
     </row>
@@ -8020,21 +8245,21 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>16:57:38</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>17:47</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -8045,12 +8270,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>18:22</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -8059,7 +8284,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -8070,23 +8295,73 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>35</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>17:47:31</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
           <t>19:04</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="C49" t="inlineStr">
         <is>
           <t>215_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D48" t="n">
-        <v>102</v>
-      </c>
-      <c r="E48" t="inlineStr">
+      <c r="D49" t="n">
+        <v>77</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>17:47:31</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>19:28</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>101</v>
+      </c>
+      <c r="E50" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8103,7 +8378,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8121,14 +8396,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:22:11</t>
+          <t>Última actualización: 17:47:31</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 38</t>
+          <t>Total filas: 39</t>
         </is>
       </c>
     </row>
@@ -8572,7 +8847,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -8597,7 +8872,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -9087,7 +9362,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -9101,11 +9376,36 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>17:47:31</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>19:24</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>97</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1301
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E273"/>
+  <dimension ref="A1:E281"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:47:31</t>
+          <t>Última actualización: 18:01:05</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 268</t>
+          <t>Total filas: 276</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1403,7 +1403,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,7 +1428,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1438,11 +1438,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2103,7 +2103,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2113,11 +2113,11 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D90" t="n">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D91" t="n">
@@ -3378,7 +3378,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>11:56:32</t>
+          <t>11:38:09</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -3388,11 +3388,11 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3403,7 +3403,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>11:38:09</t>
+          <t>11:56:32</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -3413,11 +3413,11 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3728,7 +3728,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -3738,11 +3738,11 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3763,7 +3763,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D137" t="n">
@@ -3778,7 +3778,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3788,11 +3788,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -4388,7 +4388,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D162" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4638,7 +4638,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D172" t="n">
@@ -4663,7 +4663,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D173" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D191" t="n">
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>16:57:38</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6103,7 +6103,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -6113,11 +6113,11 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6528,7 +6528,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
@@ -6542,7 +6542,7 @@
         </is>
       </c>
       <c r="D248" t="n">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -6553,7 +6553,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
@@ -6567,7 +6567,7 @@
         </is>
       </c>
       <c r="D249" t="n">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -6578,7 +6578,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -6592,7 +6592,7 @@
         </is>
       </c>
       <c r="D250" t="n">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -6603,7 +6603,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>16:49:34</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -6617,7 +6617,7 @@
         </is>
       </c>
       <c r="D251" t="n">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -6653,7 +6653,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
@@ -6667,7 +6667,7 @@
         </is>
       </c>
       <c r="D253" t="n">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -6753,7 +6753,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -6767,7 +6767,7 @@
         </is>
       </c>
       <c r="D257" t="n">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6803,7 +6803,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
@@ -6817,7 +6817,7 @@
         </is>
       </c>
       <c r="D259" t="n">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -6828,12 +6828,12 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>18:37</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
@@ -6842,7 +6842,7 @@
         </is>
       </c>
       <c r="D260" t="n">
-        <v>78</v>
+        <v>36</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -6853,21 +6853,21 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>18:41</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6878,21 +6878,21 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>18:45</t>
+          <t>18:41</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -6903,21 +6903,21 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>18:45</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -6928,21 +6928,21 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>18:57</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6953,21 +6953,21 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:57</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -6978,12 +6978,12 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
@@ -6992,7 +6992,7 @@
         </is>
       </c>
       <c r="D266" t="n">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -7003,21 +7003,21 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D267" t="n">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -7028,21 +7028,21 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D268" t="n">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -7053,21 +7053,21 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D269" t="n">
-        <v>115</v>
+        <v>69</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -7078,21 +7078,21 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>19:18</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7103,21 +7103,21 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7128,21 +7128,21 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>19:35</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7158,18 +7158,218 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
+          <t>19:18</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D273" t="n">
+        <v>91</v>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>18:01:05</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>19:23</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D274" t="n">
+        <v>82</v>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>18:01:05</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>19:28</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D275" t="n">
+        <v>87</v>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>17:47:31</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>19:35</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D276" t="n">
+        <v>108</v>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>18:01:05</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>19:36</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D277" t="n">
+        <v>95</v>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>18:01:05</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>19:39</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D278" t="n">
+        <v>98</v>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>17:47:31</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
           <t>19:40</t>
         </is>
       </c>
-      <c r="C273" t="inlineStr">
+      <c r="C279" t="inlineStr">
         <is>
           <t>15X38_ABASTO</t>
         </is>
       </c>
-      <c r="D273" t="n">
+      <c r="D279" t="n">
         <v>113</v>
       </c>
-      <c r="E273" t="inlineStr">
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>18:01:05</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>19:52</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D280" t="n">
+        <v>111</v>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>18:01:05</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>19:53</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D281" t="n">
+        <v>112</v>
+      </c>
+      <c r="E281" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7204,7 +7404,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:47:31</t>
+          <t>Última actualización: 18:01:05</t>
         </is>
       </c>
     </row>
@@ -8295,7 +8495,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -8309,7 +8509,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -8320,7 +8520,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -8334,7 +8534,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -8345,7 +8545,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -8359,7 +8559,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -8378,7 +8578,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8396,14 +8596,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:47:31</t>
+          <t>Última actualización: 18:01:05</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 39</t>
+          <t>Total filas: 40</t>
         </is>
       </c>
     </row>
@@ -9362,7 +9562,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -9376,7 +9576,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -9387,7 +9587,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -9401,11 +9601,36 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>18:01:05</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>19:58</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>117</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1302
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E281"/>
+  <dimension ref="A1:E287"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:01:05</t>
+          <t>Última actualización: 18:34:20</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 276</t>
+          <t>Total filas: 282</t>
         </is>
       </c>
     </row>
@@ -1453,7 +1453,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1463,11 +1463,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1478,7 +1478,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1488,11 +1488,11 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1938,11 +1938,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2103,7 +2103,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2113,11 +2113,11 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3263,7 +3263,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D117" t="n">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3463,7 +3463,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D125" t="n">
@@ -3488,7 +3488,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D126" t="n">
@@ -3728,7 +3728,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -3738,11 +3738,11 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3763,7 +3763,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D137" t="n">
@@ -3778,7 +3778,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3788,11 +3788,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3828,7 +3828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3838,11 +3838,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3863,11 +3863,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4053,7 +4053,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -4063,11 +4063,11 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D191" t="n">
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>16:57:38</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6103,7 +6103,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -6113,11 +6113,11 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6428,7 +6428,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6438,11 +6438,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6453,7 +6453,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
@@ -6463,11 +6463,11 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -6803,7 +6803,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
@@ -6817,7 +6817,7 @@
         </is>
       </c>
       <c r="D259" t="n">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -6853,12 +6853,12 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>18:39</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
@@ -6867,7 +6867,7 @@
         </is>
       </c>
       <c r="D261" t="n">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6878,21 +6878,21 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>18:41</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -6903,21 +6903,21 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>18:45</t>
+          <t>18:41</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -6928,21 +6928,21 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>18:45</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6953,21 +6953,21 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>18:57</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -6978,21 +6978,21 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:57</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D266" t="n">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -7003,12 +7003,12 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
@@ -7017,7 +7017,7 @@
         </is>
       </c>
       <c r="D267" t="n">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -7033,16 +7033,16 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D268" t="n">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -7053,21 +7053,21 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D269" t="n">
-        <v>69</v>
+        <v>30</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -7078,21 +7078,21 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7103,21 +7103,21 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7128,7 +7128,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -7142,7 +7142,7 @@
         </is>
       </c>
       <c r="D272" t="n">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7153,12 +7153,12 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>19:18</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
@@ -7167,7 +7167,7 @@
         </is>
       </c>
       <c r="D273" t="n">
-        <v>91</v>
+        <v>43</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -7178,12 +7178,12 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>19:23</t>
+          <t>19:18</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
@@ -7192,7 +7192,7 @@
         </is>
       </c>
       <c r="D274" t="n">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -7203,21 +7203,21 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:18</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D275" t="n">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -7228,21 +7228,21 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>19:35</t>
+          <t>19:23</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D276" t="n">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -7253,21 +7253,21 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>19:36</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7278,21 +7278,21 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:35</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7303,21 +7303,21 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:36</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D279" t="n">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -7328,21 +7328,21 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>19:52</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D280" t="n">
-        <v>111</v>
+        <v>65</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -7353,23 +7353,173 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D281" t="n">
+        <v>113</v>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>18:34:20</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>19:52</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D282" t="n">
+        <v>78</v>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>18:34:20</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
           <t>19:53</t>
         </is>
       </c>
-      <c r="C281" t="inlineStr">
+      <c r="C283" t="inlineStr">
         <is>
           <t>225_GOMEZ</t>
         </is>
       </c>
-      <c r="D281" t="n">
-        <v>112</v>
-      </c>
-      <c r="E281" t="inlineStr">
+      <c r="D283" t="n">
+        <v>79</v>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>18:34:20</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>20:07</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D284" t="n">
+        <v>93</v>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>18:34:20</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>20:12</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D285" t="n">
+        <v>98</v>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>18:34:20</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D286" t="n">
+        <v>108</v>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>18:34:20</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D287" t="n">
+        <v>117</v>
+      </c>
+      <c r="E287" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7386,7 +7536,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7404,14 +7554,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:01:05</t>
+          <t>Última actualización: 18:34:20</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 45</t>
+          <t>Total filas: 46</t>
         </is>
       </c>
     </row>
@@ -8520,7 +8670,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -8534,7 +8684,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -8545,7 +8695,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -8559,9 +8709,34 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="E50" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>18:34:20</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>20:07</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>93</v>
+      </c>
+      <c r="E51" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8596,7 +8771,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:01:05</t>
+          <t>Última actualización: 18:34:20</t>
         </is>
       </c>
     </row>
@@ -9562,7 +9737,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -9576,7 +9751,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -9587,7 +9762,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -9601,7 +9776,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -9612,7 +9787,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -9626,7 +9801,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1303
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E287"/>
+  <dimension ref="A1:E295"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:34:20</t>
+          <t>Última actualización: 18:50:27</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 282</t>
+          <t>Total filas: 290</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1403,7 +1403,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,7 +1428,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1438,11 +1438,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1453,7 +1453,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1463,11 +1463,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1478,7 +1478,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1488,11 +1488,11 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2103,7 +2103,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2113,11 +2113,11 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>10:32:07</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3263,7 +3263,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D117" t="n">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4053,7 +4053,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -4063,11 +4063,11 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4388,7 +4388,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D162" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -5303,7 +5303,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -5313,11 +5313,11 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5328,7 +5328,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -5338,11 +5338,11 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>16:57:38</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6103,7 +6103,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -6113,11 +6113,11 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6428,7 +6428,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6438,11 +6438,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6453,7 +6453,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
@@ -6463,11 +6463,11 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -6953,7 +6953,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -6967,7 +6967,7 @@
         </is>
       </c>
       <c r="D265" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -6978,21 +6978,21 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>18:57</t>
+          <t>18:53</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D266" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -7003,21 +7003,21 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:57</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D267" t="n">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -7028,12 +7028,12 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
@@ -7042,7 +7042,7 @@
         </is>
       </c>
       <c r="D268" t="n">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -7053,21 +7053,21 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D269" t="n">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -7078,21 +7078,21 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7103,21 +7103,21 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7133,16 +7133,16 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7153,12 +7153,12 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
@@ -7167,7 +7167,7 @@
         </is>
       </c>
       <c r="D273" t="n">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -7178,21 +7178,21 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>19:18</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D274" t="n">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -7203,12 +7203,12 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>19:18</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -7217,7 +7217,7 @@
         </is>
       </c>
       <c r="D275" t="n">
-        <v>91</v>
+        <v>43</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -7228,12 +7228,12 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>19:23</t>
+          <t>19:18</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -7242,7 +7242,7 @@
         </is>
       </c>
       <c r="D276" t="n">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -7253,21 +7253,21 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:18</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7278,21 +7278,21 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>19:35</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7303,21 +7303,21 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>19:36</t>
+          <t>19:23</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D279" t="n">
-        <v>95</v>
+        <v>33</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -7328,21 +7328,21 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:23</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D280" t="n">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -7353,21 +7353,21 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>113</v>
+        <v>38</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7378,21 +7378,21 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>19:52</t>
+          <t>19:35</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7403,21 +7403,21 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>19:53</t>
+          <t>19:36</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7428,21 +7428,21 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>20:07</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7453,21 +7453,21 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -7478,21 +7478,21 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>19:52</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>108</v>
+        <v>62</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,23 +7503,223 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
+          <t>18:50:27</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>19:53</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D287" t="n">
+        <v>63</v>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>18:50:27</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>20:05</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D288" t="n">
+        <v>75</v>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>18:50:27</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>20:07</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D289" t="n">
+        <v>77</v>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>18:50:27</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>20:12</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D290" t="n">
+        <v>82</v>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>18:50:27</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D291" t="n">
+        <v>92</v>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>18:50:27</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D292" t="n">
+        <v>100</v>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
           <t>18:34:20</t>
         </is>
       </c>
-      <c r="B287" t="inlineStr">
+      <c r="B293" t="inlineStr">
         <is>
           <t>20:31</t>
         </is>
       </c>
-      <c r="C287" t="inlineStr">
+      <c r="C293" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D287" t="n">
+      <c r="D293" t="n">
         <v>117</v>
       </c>
-      <c r="E287" t="inlineStr">
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>18:50:27</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>20:46</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D294" t="n">
+        <v>116</v>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>18:50:27</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>20:47</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D295" t="n">
+        <v>117</v>
+      </c>
+      <c r="E295" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7536,7 +7736,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7554,14 +7754,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:34:20</t>
+          <t>Última actualización: 18:50:27</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 46</t>
+          <t>Total filas: 47</t>
         </is>
       </c>
     </row>
@@ -8670,7 +8870,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -8684,7 +8884,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -8695,7 +8895,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -8709,7 +8909,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -8720,7 +8920,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -8734,9 +8934,34 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="E51" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>18:50:27</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>20:47</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>117</v>
+      </c>
+      <c r="E52" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8771,7 +8996,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:34:20</t>
+          <t>Última actualización: 18:50:27</t>
         </is>
       </c>
     </row>
@@ -9762,7 +9987,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -9776,7 +10001,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -9787,7 +10012,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -9801,7 +10026,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1304
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E295"/>
+  <dimension ref="A1:E304"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:50:27</t>
+          <t>Última actualización: 19:14:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 290</t>
+          <t>Total filas: 299</t>
         </is>
       </c>
     </row>
@@ -1403,7 +1403,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,7 +1428,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1438,11 +1438,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1938,11 +1938,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2103,7 +2103,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2113,11 +2113,11 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D133" t="n">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -3728,7 +3728,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -3738,11 +3738,11 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3763,7 +3763,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D137" t="n">
@@ -3778,7 +3778,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3788,11 +3788,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3828,7 +3828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3838,11 +3838,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3863,11 +3863,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4388,7 +4388,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D162" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4638,7 +4638,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D172" t="n">
@@ -4663,7 +4663,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D173" t="n">
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>16:57:38</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6103,7 +6103,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -6113,11 +6113,11 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6428,7 +6428,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6438,11 +6438,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6453,7 +6453,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
@@ -6463,11 +6463,11 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -6563,7 +6563,7 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D249" t="n">
@@ -6588,7 +6588,7 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D250" t="n">
@@ -7128,21 +7128,21 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:15</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7178,21 +7178,21 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D274" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -7203,7 +7203,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
@@ -7213,11 +7213,11 @@
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D275" t="n">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -7228,21 +7228,21 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>19:18</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D276" t="n">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -7253,7 +7253,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -7263,11 +7263,11 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>91</v>
+        <v>44</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7278,21 +7278,21 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:18</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7303,21 +7303,21 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>19:23</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D279" t="n">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -7353,21 +7353,21 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:23</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7378,21 +7378,21 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>19:35</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7403,12 +7403,12 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>19:36</t>
+          <t>19:35</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -7417,7 +7417,7 @@
         </is>
       </c>
       <c r="D283" t="n">
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7428,21 +7428,21 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:36</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7453,12 +7453,12 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -7467,7 +7467,7 @@
         </is>
       </c>
       <c r="D285" t="n">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -7478,21 +7478,21 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>19:52</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>62</v>
+        <v>113</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,21 +7503,21 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>19:53</t>
+          <t>19:52</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7528,21 +7528,21 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>20:05</t>
+          <t>19:53</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D288" t="n">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -7553,21 +7553,21 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>20:07</t>
+          <t>19:53</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7583,16 +7583,16 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>20:05</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7603,21 +7603,21 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:07</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D291" t="n">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -7628,21 +7628,21 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,21 +7653,21 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7678,21 +7678,21 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>20:46</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>116</v>
+        <v>59</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,23 +7703,248 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
+          <t>19:14:15</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D295" t="n">
+        <v>68</v>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
           <t>18:50:27</t>
         </is>
       </c>
-      <c r="B295" t="inlineStr">
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D296" t="n">
+        <v>100</v>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>19:14:15</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D297" t="n">
+        <v>77</v>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>18:50:27</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>20:46</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D298" t="n">
+        <v>116</v>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>18:50:27</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
         <is>
           <t>20:47</t>
         </is>
       </c>
-      <c r="C295" t="inlineStr">
+      <c r="C299" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D295" t="n">
+      <c r="D299" t="n">
         <v>117</v>
       </c>
-      <c r="E295" t="inlineStr">
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>19:14:15</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>20:48</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D300" t="n">
+        <v>94</v>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>19:14:15</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>20:50</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D301" t="n">
+        <v>96</v>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>19:14:15</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>20:57</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D302" t="n">
+        <v>103</v>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>19:14:15</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D303" t="n">
+        <v>113</v>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>19:14:15</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>21:10</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D304" t="n">
+        <v>116</v>
+      </c>
+      <c r="E304" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7736,7 +7961,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7754,14 +7979,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:50:27</t>
+          <t>Última actualización: 19:14:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 47</t>
+          <t>Total filas: 48</t>
         </is>
       </c>
     </row>
@@ -8895,7 +9120,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -8909,7 +9134,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -8920,7 +9145,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -8934,7 +9159,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -8962,6 +9187,31 @@
         <v>117</v>
       </c>
       <c r="E52" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>19:14:15</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>20:48</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>94</v>
+      </c>
+      <c r="E53" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8978,7 +9228,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8996,14 +9246,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:50:27</t>
+          <t>Última actualización: 19:14:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 40</t>
+          <t>Total filas: 41</t>
         </is>
       </c>
     </row>
@@ -9987,7 +10237,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -10001,7 +10251,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -10012,7 +10262,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -10026,9 +10276,34 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="E45" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>19:14:15</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>98</v>
+      </c>
+      <c r="E46" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1305
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E304"/>
+  <dimension ref="A1:E311"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:14:15</t>
+          <t>Última actualización: 19:45:00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 299</t>
+          <t>Total filas: 306</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1403,7 +1403,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,7 +1428,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1438,11 +1438,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1938,11 +1938,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D90" t="n">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D91" t="n">
@@ -3663,7 +3663,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -3728,7 +3728,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -3738,11 +3738,11 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3778,7 +3778,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3788,11 +3788,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D191" t="n">
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6103,7 +6103,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -6113,11 +6113,11 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6428,7 +6428,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6438,11 +6438,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6453,7 +6453,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
@@ -6463,11 +6463,11 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -7153,7 +7153,7 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
@@ -7163,11 +7163,11 @@
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D273" t="n">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -7178,7 +7178,7 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
@@ -7188,11 +7188,11 @@
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D274" t="n">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -7328,7 +7328,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
@@ -7338,11 +7338,11 @@
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D280" t="n">
-        <v>82</v>
+        <v>9</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -7353,7 +7353,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -7363,11 +7363,11 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7503,7 +7503,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>19:45:00</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -7517,7 +7517,7 @@
         </is>
       </c>
       <c r="D287" t="n">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7528,7 +7528,7 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>19:45:00</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
@@ -7538,11 +7538,11 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D288" t="n">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -7553,7 +7553,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>19:45:00</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7563,11 +7563,11 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7603,7 +7603,7 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>19:45:00</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
@@ -7617,7 +7617,7 @@
         </is>
       </c>
       <c r="D291" t="n">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -7628,12 +7628,12 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>19:45:00</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -7642,7 +7642,7 @@
         </is>
       </c>
       <c r="D292" t="n">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,21 +7653,21 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7678,12 +7678,12 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -7692,7 +7692,7 @@
         </is>
       </c>
       <c r="D294" t="n">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,21 +7703,21 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>19:45:00</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7728,21 +7728,21 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:45:00</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -7753,12 +7753,12 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -7767,7 +7767,7 @@
         </is>
       </c>
       <c r="D297" t="n">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7778,21 +7778,21 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:45:00</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>20:46</t>
+          <t>20:31</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D298" t="n">
-        <v>116</v>
+        <v>46</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -7803,21 +7803,21 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:45:00</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>20:47</t>
+          <t>20:34</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D299" t="n">
-        <v>117</v>
+        <v>49</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -7828,21 +7828,21 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>20:48</t>
+          <t>20:46</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D300" t="n">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -7853,21 +7853,21 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>20:50</t>
+          <t>20:47</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7878,21 +7878,21 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>19:45:00</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:48</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7908,16 +7908,16 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>20:50</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -7928,23 +7928,198 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
+          <t>19:45:00</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D304" t="n">
+        <v>67</v>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>19:45:00</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>20:55</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D305" t="n">
+        <v>70</v>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>19:45:00</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D306" t="n">
+        <v>71</v>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
           <t>19:14:15</t>
         </is>
       </c>
-      <c r="B304" t="inlineStr">
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>20:57</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D307" t="n">
+        <v>103</v>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>19:45:00</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D308" t="n">
+        <v>82</v>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>19:45:00</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
         <is>
           <t>21:10</t>
         </is>
       </c>
-      <c r="C304" t="inlineStr">
+      <c r="C309" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D304" t="n">
-        <v>116</v>
-      </c>
-      <c r="E304" t="inlineStr">
+      <c r="D309" t="n">
+        <v>85</v>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>19:45:00</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>21:28</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D310" t="n">
+        <v>103</v>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>19:45:00</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>21:34</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D311" t="n">
+        <v>109</v>
+      </c>
+      <c r="E311" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7979,7 +8154,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:14:15</t>
+          <t>Última actualización: 19:45:00</t>
         </is>
       </c>
     </row>
@@ -9145,7 +9320,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>19:45:00</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -9159,7 +9334,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -9195,7 +9370,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>19:45:00</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -9209,7 +9384,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -9246,7 +9421,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:14:15</t>
+          <t>Última actualización: 19:45:00</t>
         </is>
       </c>
     </row>
@@ -10262,7 +10437,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>19:45:00</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -10276,7 +10451,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -10287,7 +10462,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>19:45:00</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -10301,7 +10476,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1306
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E311"/>
+  <dimension ref="A1:E316"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:45:00</t>
+          <t>Última actualización: 20:00:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 306</t>
+          <t>Total filas: 311</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -903,7 +903,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -913,11 +913,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -938,11 +938,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1703,7 +1703,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1713,11 +1713,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1938,11 +1938,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2103,7 +2103,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2113,11 +2113,11 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D90" t="n">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D91" t="n">
@@ -3828,7 +3828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3838,11 +3838,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3863,11 +3863,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4053,7 +4053,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -4063,11 +4063,11 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D172" t="n">
@@ -4663,7 +4663,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D173" t="n">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D191" t="n">
@@ -5138,7 +5138,7 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D192" t="n">
@@ -5303,7 +5303,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -5313,11 +5313,11 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5328,7 +5328,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -5338,11 +5338,11 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>16:57:38</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -6563,7 +6563,7 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D249" t="n">
@@ -6588,7 +6588,7 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D250" t="n">
@@ -7328,7 +7328,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
@@ -7338,11 +7338,11 @@
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D280" t="n">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -7353,7 +7353,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -7363,11 +7363,11 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>82</v>
+        <v>9</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7603,7 +7603,7 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>19:45:00</t>
+          <t>20:00:07</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
@@ -7617,7 +7617,7 @@
         </is>
       </c>
       <c r="D291" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -7628,12 +7628,12 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>19:45:00</t>
+          <t>20:00:07</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>20:08</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -7642,7 +7642,7 @@
         </is>
       </c>
       <c r="D292" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,12 +7653,12 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>19:45:00</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -7667,7 +7667,7 @@
         </is>
       </c>
       <c r="D293" t="n">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7678,21 +7678,21 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,12 +7703,12 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>19:45:00</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -7717,7 +7717,7 @@
         </is>
       </c>
       <c r="D295" t="n">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7728,21 +7728,21 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>19:45:00</t>
+          <t>20:00:07</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -7753,21 +7753,21 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>20:00:07</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7778,12 +7778,12 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>19:45:00</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -7792,7 +7792,7 @@
         </is>
       </c>
       <c r="D298" t="n">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -7803,21 +7803,21 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>19:45:00</t>
+          <t>20:00:07</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>20:34</t>
+          <t>20:31</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D299" t="n">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -7828,21 +7828,21 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>20:00:07</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>20:46</t>
+          <t>20:34</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D300" t="n">
-        <v>116</v>
+        <v>34</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -7853,21 +7853,21 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>20:00:07</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>20:47</t>
+          <t>20:46</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>117</v>
+        <v>46</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7878,12 +7878,12 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>19:45:00</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>20:48</t>
+          <t>20:47</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -7892,7 +7892,7 @@
         </is>
       </c>
       <c r="D302" t="n">
-        <v>63</v>
+        <v>117</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7903,21 +7903,21 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>20:00:07</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>20:50</t>
+          <t>20:48</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -7928,12 +7928,12 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>19:45:00</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:50</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -7942,7 +7942,7 @@
         </is>
       </c>
       <c r="D304" t="n">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -7958,16 +7958,16 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>20:55</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D305" t="n">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -7983,16 +7983,16 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:55</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -8003,12 +8003,12 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>19:45:00</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -8017,7 +8017,7 @@
         </is>
       </c>
       <c r="D307" t="n">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,21 +8028,21 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>19:45:00</t>
+          <t>20:00:07</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8053,21 +8053,21 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>19:45:00</t>
+          <t>20:00:07</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>21:10</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,21 +8078,21 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>19:45:00</t>
+          <t>20:00:07</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>21:10</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8108,18 +8108,143 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
+          <t>21:28</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D311" t="n">
+        <v>103</v>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>20:00:07</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D312" t="n">
+        <v>89</v>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>20:00:07</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>21:33</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D313" t="n">
+        <v>93</v>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>20:00:07</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
           <t>21:34</t>
         </is>
       </c>
-      <c r="C311" t="inlineStr">
+      <c r="C314" t="inlineStr">
         <is>
           <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
-      <c r="D311" t="n">
-        <v>109</v>
-      </c>
-      <c r="E311" t="inlineStr">
+      <c r="D314" t="n">
+        <v>94</v>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>20:00:07</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>21:46</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D315" t="n">
+        <v>106</v>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>20:00:07</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>21:48</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D316" t="n">
+        <v>108</v>
+      </c>
+      <c r="E316" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8154,7 +8279,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:45:00</t>
+          <t>Última actualización: 20:00:07</t>
         </is>
       </c>
     </row>
@@ -9320,7 +9445,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>19:45:00</t>
+          <t>20:00:07</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -9334,7 +9459,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -9370,7 +9495,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>19:45:00</t>
+          <t>20:00:07</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -9384,7 +9509,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -9403,7 +9528,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9421,14 +9546,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:45:00</t>
+          <t>Última actualización: 20:00:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 41</t>
+          <t>Total filas: 42</t>
         </is>
       </c>
     </row>
@@ -10462,23 +10587,48 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>19:45:00</t>
+          <t>20:00:07</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>20:00:07</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
           <t>20:52</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="C47" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D46" t="n">
-        <v>67</v>
-      </c>
-      <c r="E46" t="inlineStr">
+      <c r="D47" t="n">
+        <v>52</v>
+      </c>
+      <c r="E47" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1307
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E316"/>
+  <dimension ref="A1:E320"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:00:07</t>
+          <t>Última actualización: 20:28:23</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 311</t>
+          <t>Total filas: 315</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -903,7 +903,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -913,11 +913,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -938,11 +938,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -2103,7 +2103,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2113,11 +2113,11 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>10:32:07</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3263,7 +3263,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D117" t="n">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3663,7 +3663,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D133" t="n">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -3828,7 +3828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3838,11 +3838,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3863,11 +3863,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5138,7 +5138,7 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D192" t="n">
@@ -5303,7 +5303,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -5313,11 +5313,11 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5328,7 +5328,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -5338,11 +5338,11 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -7328,7 +7328,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
@@ -7338,11 +7338,11 @@
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D280" t="n">
-        <v>82</v>
+        <v>9</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -7353,7 +7353,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -7363,11 +7363,11 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7803,7 +7803,7 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>20:00:07</t>
+          <t>20:28:23</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
@@ -7817,7 +7817,7 @@
         </is>
       </c>
       <c r="D299" t="n">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -7828,7 +7828,7 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>20:00:07</t>
+          <t>20:28:23</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
@@ -7842,7 +7842,7 @@
         </is>
       </c>
       <c r="D300" t="n">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -7853,7 +7853,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>20:00:07</t>
+          <t>20:28:23</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -7867,7 +7867,7 @@
         </is>
       </c>
       <c r="D301" t="n">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7878,7 +7878,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>20:28:23</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -7892,7 +7892,7 @@
         </is>
       </c>
       <c r="D302" t="n">
-        <v>117</v>
+        <v>19</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7978,7 +7978,7 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>19:45:00</t>
+          <t>20:28:23</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
@@ -7992,7 +7992,7 @@
         </is>
       </c>
       <c r="D306" t="n">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -8028,7 +8028,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>20:00:07</t>
+          <t>20:28:23</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8042,7 +8042,7 @@
         </is>
       </c>
       <c r="D308" t="n">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>20:00:07</t>
+          <t>20:28:23</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8067,7 +8067,7 @@
         </is>
       </c>
       <c r="D309" t="n">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,7 +8078,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>20:00:07</t>
+          <t>20:28:23</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8092,7 +8092,7 @@
         </is>
       </c>
       <c r="D310" t="n">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8103,7 +8103,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>19:45:00</t>
+          <t>20:28:23</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
@@ -8117,7 +8117,7 @@
         </is>
       </c>
       <c r="D311" t="n">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8178,7 +8178,7 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>20:00:07</t>
+          <t>20:28:23</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
@@ -8192,7 +8192,7 @@
         </is>
       </c>
       <c r="D314" t="n">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -8203,21 +8203,21 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>20:00:07</t>
+          <t>20:28:23</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>21:34</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8228,23 +8228,123 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
+          <t>20:28:23</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>21:45</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D316" t="n">
+        <v>77</v>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>20:28:23</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>21:46</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D317" t="n">
+        <v>78</v>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
           <t>20:00:07</t>
         </is>
       </c>
-      <c r="B316" t="inlineStr">
+      <c r="B318" t="inlineStr">
         <is>
           <t>21:48</t>
         </is>
       </c>
-      <c r="C316" t="inlineStr">
+      <c r="C318" t="inlineStr">
         <is>
           <t>23_HERNANDEZ</t>
         </is>
       </c>
-      <c r="D316" t="n">
+      <c r="D318" t="n">
         <v>108</v>
       </c>
-      <c r="E316" t="inlineStr">
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>20:28:23</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>22:04</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D319" t="n">
+        <v>96</v>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>20:28:23</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>22:11</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D320" t="n">
+        <v>103</v>
+      </c>
+      <c r="E320" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8279,7 +8379,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:00:07</t>
+          <t>Última actualización: 20:28:23</t>
         </is>
       </c>
     </row>
@@ -9470,7 +9570,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>20:28:23</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -9484,7 +9584,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>117</v>
+        <v>19</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -9528,7 +9628,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9546,14 +9646,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:00:07</t>
+          <t>Última actualización: 20:28:23</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 42</t>
+          <t>Total filas: 44</t>
         </is>
       </c>
     </row>
@@ -10612,7 +10712,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>20:00:07</t>
+          <t>20:28:23</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -10626,11 +10726,61 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>20:28:23</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>21:30</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>62</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>20:28:23</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>22:20</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>112</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1308
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E320"/>
+  <dimension ref="A1:E325"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:28:23</t>
+          <t>Última actualización: 20:48:26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 315</t>
+          <t>Total filas: 320</t>
         </is>
       </c>
     </row>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D90" t="n">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D91" t="n">
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>10:32:07</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3263,7 +3263,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D117" t="n">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3463,7 +3463,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D125" t="n">
@@ -3488,7 +3488,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D126" t="n">
@@ -3663,7 +3663,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -3728,7 +3728,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -3738,11 +3738,11 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3763,7 +3763,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D137" t="n">
@@ -3778,7 +3778,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3788,11 +3788,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3828,7 +3828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3838,11 +3838,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3863,11 +3863,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5303,7 +5303,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -5313,11 +5313,11 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5328,7 +5328,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -5338,11 +5338,11 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6103,7 +6103,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -6113,11 +6113,11 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -7328,7 +7328,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
@@ -7338,11 +7338,11 @@
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D280" t="n">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -7353,7 +7353,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -7363,11 +7363,11 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>82</v>
+        <v>9</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7903,7 +7903,7 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>20:00:07</t>
+          <t>20:48:26</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
@@ -7917,7 +7917,7 @@
         </is>
       </c>
       <c r="D303" t="n">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -7928,12 +7928,12 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>20:48:26</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>20:50</t>
+          <t>20:49</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -7942,7 +7942,7 @@
         </is>
       </c>
       <c r="D304" t="n">
-        <v>96</v>
+        <v>1</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -7953,12 +7953,12 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>19:45:00</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:50</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -7967,7 +7967,7 @@
         </is>
       </c>
       <c r="D305" t="n">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -7978,21 +7978,21 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>20:28:23</t>
+          <t>19:45:00</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>20:55</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -8003,21 +8003,21 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>19:45:00</t>
+          <t>20:48:26</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:55</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,12 +8028,12 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>20:28:23</t>
+          <t>20:48:26</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -8042,7 +8042,7 @@
         </is>
       </c>
       <c r="D308" t="n">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8058,16 +8058,16 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,21 +8078,21 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>20:28:23</t>
+          <t>20:48:26</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>21:10</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8103,21 +8103,21 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>20:28:23</t>
+          <t>20:48:26</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>21:10</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D311" t="n">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8128,12 +8128,12 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>20:00:07</t>
+          <t>20:48:26</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -8142,7 +8142,7 @@
         </is>
       </c>
       <c r="D312" t="n">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -8158,16 +8158,16 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>21:33</t>
+          <t>21:29</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D313" t="n">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -8178,21 +8178,21 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>20:28:23</t>
+          <t>20:00:07</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>21:34</t>
+          <t>21:33</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D314" t="n">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -8203,7 +8203,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>20:28:23</t>
+          <t>20:48:26</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
@@ -8213,11 +8213,11 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8228,21 +8228,21 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>20:28:23</t>
+          <t>20:48:26</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>21:34</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8258,16 +8258,16 @@
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>21:45</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D317" t="n">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
@@ -8278,21 +8278,21 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>20:00:07</t>
+          <t>20:48:26</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>21:48</t>
+          <t>21:46</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D318" t="n">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -8303,21 +8303,21 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>20:28:23</t>
+          <t>20:00:07</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>22:04</t>
+          <t>21:48</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D319" t="n">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -8328,23 +8328,148 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>20:28:23</t>
+          <t>20:48:26</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
+          <t>21:55</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D320" t="n">
+        <v>67</v>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>20:48:26</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>22:04</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D321" t="n">
+        <v>76</v>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>20:48:26</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
           <t>22:11</t>
         </is>
       </c>
-      <c r="C320" t="inlineStr">
+      <c r="C322" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D320" t="n">
-        <v>103</v>
-      </c>
-      <c r="E320" t="inlineStr">
+      <c r="D322" t="n">
+        <v>83</v>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>20:48:26</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>22:33</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D323" t="n">
+        <v>105</v>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>20:48:26</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>22:34</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D324" t="n">
+        <v>106</v>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>20:48:26</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>22:43</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D325" t="n">
+        <v>115</v>
+      </c>
+      <c r="E325" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8361,7 +8486,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8379,14 +8504,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:28:23</t>
+          <t>Última actualización: 20:48:26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 48</t>
+          <t>Total filas: 49</t>
         </is>
       </c>
     </row>
@@ -9595,7 +9720,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>20:00:07</t>
+          <t>20:48:26</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -9609,9 +9734,34 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="E53" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>20:48:26</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>22:33</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>105</v>
+      </c>
+      <c r="E54" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9628,7 +9778,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9646,14 +9796,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:28:23</t>
+          <t>Última actualización: 20:48:26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 44</t>
+          <t>Total filas: 45</t>
         </is>
       </c>
     </row>
@@ -10012,7 +10162,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -10022,11 +10172,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>101</v>
+        <v>48</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -10037,7 +10187,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>09:42:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -10047,11 +10197,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -10737,12 +10887,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>20:28:23</t>
+          <t>20:48:26</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>21:30</t>
+          <t>20:54</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -10751,7 +10901,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -10762,23 +10912,48 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>20:28:23</t>
+          <t>20:48:26</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
+          <t>21:30</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>42</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>20:48:26</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
           <t>22:20</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="C50" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D49" t="n">
-        <v>112</v>
-      </c>
-      <c r="E49" t="inlineStr">
+      <c r="D50" t="n">
+        <v>92</v>
+      </c>
+      <c r="E50" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1309
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E325"/>
+  <dimension ref="A1:E333"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:48:26</t>
+          <t>Última actualización: 20:59:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 320</t>
+          <t>Total filas: 328</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -903,7 +903,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -913,11 +913,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -938,11 +938,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1203,7 +1203,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1213,11 +1213,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1228,7 +1228,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1238,11 +1238,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,7 +1428,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1438,11 +1438,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2103,7 +2103,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2113,11 +2113,11 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,7 +2128,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>10:32:07</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2928,7 +2928,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2938,11 +2938,11 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3463,7 +3463,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D125" t="n">
@@ -3488,7 +3488,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D126" t="n">
@@ -3738,7 +3738,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D136" t="n">
@@ -3753,7 +3753,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -3763,11 +3763,11 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3778,7 +3778,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3788,11 +3788,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -4028,7 +4028,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4038,11 +4038,11 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4053,7 +4053,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -4063,11 +4063,11 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4103,7 +4103,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4113,11 +4113,11 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D172" t="n">
@@ -4663,7 +4663,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D173" t="n">
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D191" t="n">
@@ -5138,7 +5138,7 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D192" t="n">
@@ -5303,7 +5303,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -5313,11 +5313,11 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5328,7 +5328,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -5338,11 +5338,11 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -5903,7 +5903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>16:57:38</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>17:22:11</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6103,7 +6103,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>17:22:11</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -6113,11 +6113,11 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -7203,7 +7203,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
@@ -7213,11 +7213,11 @@
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D275" t="n">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -7228,7 +7228,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
@@ -7238,11 +7238,11 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D276" t="n">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -7253,7 +7253,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>17:47:31</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -7263,11 +7263,11 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7278,7 +7278,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>17:47:31</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -7288,11 +7288,11 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>91</v>
+        <v>44</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7328,7 +7328,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>18:01:05</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
@@ -7338,11 +7338,11 @@
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D280" t="n">
-        <v>82</v>
+        <v>9</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -7353,7 +7353,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>18:01:05</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -7363,11 +7363,11 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -8078,12 +8078,12 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>20:48:26</t>
+          <t>20:59:52</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>21:06</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -8092,7 +8092,7 @@
         </is>
       </c>
       <c r="D310" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8108,16 +8108,16 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>21:10</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D311" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8128,21 +8128,21 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>20:48:26</t>
+          <t>20:59:52</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>21:09</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D312" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -8153,21 +8153,21 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>20:00:07</t>
+          <t>20:48:26</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>21:10</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D313" t="n">
-        <v>89</v>
+        <v>22</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -8178,21 +8178,21 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>20:00:07</t>
+          <t>20:59:52</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>21:33</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D314" t="n">
-        <v>93</v>
+        <v>29</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -8203,21 +8203,21 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>20:48:26</t>
+          <t>20:00:07</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>21:34</t>
+          <t>21:29</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8228,21 +8228,21 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>20:48:26</t>
+          <t>20:59:52</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>21:34</t>
+          <t>21:33</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8253,21 +8253,21 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>20:28:23</t>
+          <t>20:59:52</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>21:45</t>
+          <t>21:33</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D317" t="n">
-        <v>77</v>
+        <v>34</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
@@ -8283,16 +8283,16 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>21:34</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D318" t="n">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -8303,21 +8303,21 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>20:00:07</t>
+          <t>20:48:26</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>21:48</t>
+          <t>21:34</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D319" t="n">
-        <v>108</v>
+        <v>46</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -8328,21 +8328,21 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>20:48:26</t>
+          <t>20:59:52</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>21:55</t>
+          <t>21:45</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -8353,21 +8353,21 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>20:48:26</t>
+          <t>20:28:23</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>22:04</t>
+          <t>21:45</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D321" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -8383,16 +8383,16 @@
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>22:11</t>
+          <t>21:46</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D322" t="n">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -8403,21 +8403,21 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>20:48:26</t>
+          <t>20:00:07</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>22:33</t>
+          <t>21:48</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8428,21 +8428,21 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>20:48:26</t>
+          <t>20:59:52</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>22:34</t>
+          <t>21:55</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8453,23 +8453,223 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
+          <t>20:59:52</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>22:03</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D325" t="n">
+        <v>64</v>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
           <t>20:48:26</t>
         </is>
       </c>
-      <c r="B325" t="inlineStr">
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>22:04</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D326" t="n">
+        <v>76</v>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>20:59:52</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>22:10</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D327" t="n">
+        <v>71</v>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>20:48:26</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>22:11</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D328" t="n">
+        <v>83</v>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>20:59:52</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>22:33</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D329" t="n">
+        <v>94</v>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>20:59:52</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>22:33</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D330" t="n">
+        <v>94</v>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>20:59:52</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>22:34</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D331" t="n">
+        <v>95</v>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>20:48:26</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>22:34</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D332" t="n">
+        <v>106</v>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>20:59:52</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
         <is>
           <t>22:43</t>
         </is>
       </c>
-      <c r="C325" t="inlineStr">
+      <c r="C333" t="inlineStr">
         <is>
           <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D325" t="n">
-        <v>115</v>
-      </c>
-      <c r="E325" t="inlineStr">
+      <c r="D333" t="n">
+        <v>104</v>
+      </c>
+      <c r="E333" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8504,7 +8704,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:48:26</t>
+          <t>Última actualización: 20:59:52</t>
         </is>
       </c>
     </row>
@@ -9745,7 +9945,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>20:48:26</t>
+          <t>20:59:52</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -9759,7 +9959,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -9778,7 +9978,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9796,14 +9996,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:48:26</t>
+          <t>Última actualización: 20:59:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 45</t>
+          <t>Total filas: 47</t>
         </is>
       </c>
     </row>
@@ -10162,7 +10362,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>09:42:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -10172,11 +10372,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -10187,7 +10387,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -10197,11 +10397,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>101</v>
+        <v>48</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -10912,12 +11112,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>20:48:26</t>
+          <t>20:59:52</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>21:30</t>
+          <t>21:29</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -10926,7 +11126,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -10942,18 +11142,68 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
+          <t>21:30</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>42</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>20:59:52</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>22:19</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>80</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>20:48:26</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
           <t>22:20</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C52" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D50" t="n">
+      <c r="D52" t="n">
         <v>92</v>
       </c>
-      <c r="E50" t="inlineStr">
+      <c r="E52" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1310
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-02-01.xlsx
+++ b/data/horarios-141-2026-02-01.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E333"/>
+  <dimension ref="A1:E337"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:59:52</t>
+          <t>Última actualización: 23:30:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 328</t>
+          <t>Total filas: 332</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -903,7 +903,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:46:40</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -913,11 +913,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>06:46:40</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -938,11 +938,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1203,7 +1203,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>07:51:40</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1213,11 +1213,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1228,7 +1228,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>07:51:40</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1238,11 +1238,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>06:58:58</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,7 +1428,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>06:58:58</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1438,11 +1438,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1938,11 +1938,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1953,7 +1953,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1988,11 +1988,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2013,11 +2013,11 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -3463,7 +3463,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D125" t="n">
@@ -3488,7 +3488,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D126" t="n">
@@ -3753,7 +3753,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:43:13</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -3763,11 +3763,11 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3778,7 +3778,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>12:43:13</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3788,11 +3788,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5003,7 +5003,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>15:34:15</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5013,11 +5013,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>15:34:15</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5113,7 +5113,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D191" t="n">
@@ -5138,7 +5138,7 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D192" t="n">
@@ -5303,7 +5303,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -5313,11 +5313,11 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5328,7 +5328,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -5338,11 +5338,11 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -7153,7 +7153,7 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
@@ -7163,11 +7163,11 @@
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D273" t="n">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -7178,7 +7178,7 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
@@ -7188,11 +7188,11 @@
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D274" t="n">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -7203,7 +7203,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>18:50:27</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
@@ -7213,11 +7213,11 @@
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D275" t="n">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -7228,7 +7228,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>18:50:27</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
@@ -7238,11 +7238,11 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D276" t="n">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -7538,7 +7538,7 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D288" t="n">
@@ -7563,7 +7563,7 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D289" t="n">
@@ -8288,7 +8288,7 @@
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D318" t="n">
@@ -8313,7 +8313,7 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D319" t="n">
@@ -8563,7 +8563,7 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D329" t="n">
@@ -8588,7 +8588,7 @@
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D330" t="n">
@@ -8670,6 +8670,106 @@
         <v>104</v>
       </c>
       <c r="E333" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>23:30:38</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>23:34</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D334" t="n">
+        <v>4</v>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>23:30:38</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>23:39</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D335" t="n">
+        <v>9</v>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>23:30:38</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>23:54</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D336" t="n">
+        <v>24</v>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>23:30:38</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>23:58</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D337" t="n">
+        <v>28</v>
+      </c>
+      <c r="E337" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8686,7 +8786,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8704,14 +8804,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:59:52</t>
+          <t>Última actualización: 23:30:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 49</t>
+          <t>Total filas: 50</t>
         </is>
       </c>
     </row>
@@ -9962,6 +10062,31 @@
         <v>94</v>
       </c>
       <c r="E54" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>23:30:38</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>23:39</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>9</v>
+      </c>
+      <c r="E55" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9978,7 +10103,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9996,14 +10121,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:59:52</t>
+          <t>Última actualización: 23:30:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 47</t>
+          <t>Total filas: 48</t>
         </is>
       </c>
     </row>
@@ -10037,21 +10162,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>07:26:49</t>
+          <t>23:30:38</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>07:42</t>
+          <t>00:46</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -10062,12 +10187,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>06:15:23</t>
+          <t>07:26:49</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>07:43</t>
+          <t>07:42</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -10076,7 +10201,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -10087,12 +10212,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>06:15:23</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>08:35</t>
+          <t>07:43</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -10101,7 +10226,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -10112,12 +10237,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>08:36</t>
+          <t>08:35</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -10126,7 +10251,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -10137,37 +10262,37 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>08:14:55</t>
+          <t>08:35:17</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>08:50</t>
+          <t>08:36</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>08:35:17</t>
+          <t>08:14:55</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>08:51</t>
+          <t>08:50</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -10176,7 +10301,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -10187,12 +10312,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:35:17</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>08:52</t>
+          <t>08:51</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -10201,7 +10326,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -10212,12 +10337,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>08:57:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>08:59</t>
+          <t>08:52</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -10226,7 +10351,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -10242,32 +10367,32 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>09:20</t>
+          <t>08:59</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>08:57:42</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:20</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -10276,7 +10401,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -10287,37 +10412,37 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>09:42:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>10:12</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>10:13</t>
+          <t>10:12</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -10326,7 +10451,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>84</v>
+        <v>30</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -10337,37 +10462,37 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>09:42:42</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>10:29</t>
+          <t>10:13</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>08:49:06</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>10:30</t>
+          <t>10:29</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -10376,7 +10501,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>101</v>
+        <v>47</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -10417,16 +10542,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>10:31</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -10437,12 +10562,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>10:32:07</t>
+          <t>08:49:06</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>10:32</t>
+          <t>10:31</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -10451,7 +10576,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -10487,37 +10612,37 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>09:42:42</t>
+          <t>10:32:07</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>11:25</t>
+          <t>10:32</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>103</v>
+        <v>0</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>11:01:19</t>
+          <t>09:42:42</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>11:26</t>
+          <t>11:25</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -10526,7 +10651,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -10537,12 +10662,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>11:01:19</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>13:11</t>
+          <t>11:26</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -10551,7 +10676,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -10562,12 +10687,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>13:12</t>
+          <t>13:11</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -10576,7 +10701,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -10587,37 +10712,37 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>12:18:38</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>13:20</t>
+          <t>13:12</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>12:58:23</t>
+          <t>12:18:38</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>13:20</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -10626,7 +10751,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -10637,37 +10762,37 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>12:58:23</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>13:56</t>
+          <t>13:21</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>13:28:27</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>13:57</t>
+          <t>13:56</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -10676,7 +10801,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -10687,12 +10812,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>13:54:35</t>
+          <t>13:28:27</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>14:26</t>
+          <t>13:57</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -10701,7 +10826,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -10712,12 +10837,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>13:54:35</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>14:27</t>
+          <t>14:26</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -10726,7 +10851,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -10737,37 +10862,37 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>15:21</t>
+          <t>14:27</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>14:17:13</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>15:22</t>
+          <t>15:21</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -10776,7 +10901,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -10787,37 +10912,37 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>14:58:38</t>
+          <t>14:17:13</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>16:01</t>
+          <t>15:22</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>14:58:38</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>16:02</t>
+          <t>16:01</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -10826,7 +10951,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -10837,37 +10962,37 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>14:44:54</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>16:29</t>
+          <t>16:02</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>16:02:30</t>
+          <t>14:44:54</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:29</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -10876,7 +11001,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>28</v>
+        <v>105</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -10887,37 +11012,37 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>16:57:38</t>
+          <t>16:02:30</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>17:05</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>16:34:05</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>17:06</t>
+          <t>17:05</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -10926,7 +11051,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -10937,12 +11062,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>16:57:38</t>
+          <t>16:34:05</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>17:06</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -10951,7 +11076,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>98</v>
+        <v>32</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -10962,12 +11087,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>18:34:20</t>
+          <t>16:57:38</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>18:36</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -10976,7 +11101,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -10987,62 +11112,62 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>19:14:15</t>
+          <t>18:34:20</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>19:24</t>
+          <t>18:36</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>19:45:00</t>
+          <t>19:14:15</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>19:58</t>
+          <t>19:24</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>20:00:07</t>
+          <t>19:45:00</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>19:58</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -11051,7 +11176,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -11062,12 +11187,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>20:28:23</t>
+          <t>20:00:07</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -11076,7 +11201,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -11087,12 +11212,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>20:48:26</t>
+          <t>20:28:23</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>20:54</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -11101,7 +11226,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -11112,12 +11237,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>20:59:52</t>
+          <t>20:48:26</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>20:54</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -11126,7 +11251,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -11137,12 +11262,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>20:48:26</t>
+          <t>20:59:52</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>21:30</t>
+          <t>21:29</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -11151,7 +11276,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -11162,48 +11287,73 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>20:59:52</t>
+          <t>20:48:26</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>22:19</t>
+          <t>21:30</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
+          <t>20:59:52</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>22:19</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>80</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
           <t>20:48:26</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
+      <c r="B53" t="inlineStr">
         <is>
           <t>22:20</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="C53" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D52" t="n">
+      <c r="D53" t="n">
         <v>92</v>
       </c>
-      <c r="E52" t="inlineStr">
+      <c r="E53" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>